<commit_message>
fix: Sistemata compilazione report e rigenerazioni file
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SPEITSRL/SPE.IT s.r.l/FSE INI Adapter/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111SPEITSRL/SPE.IT s.r.l/FSE INI Adapter/1.0/report-checklist.xlsx
@@ -333,16 +333,16 @@
 </t>
   </si>
   <si>
-    <t>01/08/2023</t>
-  </si>
-  <si>
-    <t>2023-08-01T10:28:02+02:00</t>
-  </si>
-  <si>
-    <t>956286c91c7e71fb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.f8735f7065^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>02/08/2023</t>
+  </si>
+  <si>
+    <t>2023-08-02T17:56:28+02:00</t>
+  </si>
+  <si>
+    <t>a61b9d5076a638d0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.5a6f3098d9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -363,13 +363,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-01T10:28:05+02:00</t>
-  </si>
-  <si>
-    <t>f14aac6ca980c391</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.52a57f427c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:56:45+02:00</t>
+  </si>
+  <si>
+    <t>ce55c4b3da3067f6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.f5df58baa1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT3</t>
@@ -381,13 +381,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-01T10:28:06+02:00</t>
-  </si>
-  <si>
-    <t>7cfa15080da40709</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.0b5933cca4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:56:47+02:00</t>
+  </si>
+  <si>
+    <t>5865ccb7d18d14cd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.8a2d98fa4c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT4</t>
@@ -399,13 +399,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-01T10:28:08+02:00</t>
-  </si>
-  <si>
-    <t>e1d3aca24b4367d2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a9264f4c56^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:56:48+02:00</t>
+  </si>
+  <si>
+    <t>5bc6e2450dff7da6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.6f4ddae6f4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT5</t>
@@ -417,13 +417,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-01T10:28:10+02:00</t>
-  </si>
-  <si>
-    <t>f281c8c2847fdc78</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.c91e70c160^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:56:50+02:00</t>
+  </si>
+  <si>
+    <t>7b373dc685e91191</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.8827466ab8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>LDO</t>
@@ -437,13 +437,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:12+02:00</t>
-  </si>
-  <si>
-    <t>6540816b4237c2fd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.1043b85ed0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:56:52+02:00</t>
+  </si>
+  <si>
+    <t>09d3642d20f2fadc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.e15b237bd2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT2</t>
@@ -454,13 +454,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:13+02:00</t>
-  </si>
-  <si>
-    <t>bb4880155b80cdfb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.9a9934d7f6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:56:54+02:00</t>
+  </si>
+  <si>
+    <t>9043852718eac292</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.e35aa06c53^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT3</t>
@@ -471,13 +471,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:15+02:00</t>
-  </si>
-  <si>
-    <t>856a97c1138788cb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.16f4df6460^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:56:56+02:00</t>
+  </si>
+  <si>
+    <t>f606b8d380a7fc6e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.94dd5c9716^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT4</t>
@@ -488,13 +488,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:17+02:00</t>
-  </si>
-  <si>
-    <t>0893114b241a9125</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.f45eaab27d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:56:58+02:00</t>
+  </si>
+  <si>
+    <t>0e88eca633171ebb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.ab3c47553a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>RAD</t>
@@ -508,13 +508,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:19+02:00</t>
-  </si>
-  <si>
-    <t>bc154172ac2a9921</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.979005073b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:56:59+02:00</t>
+  </si>
+  <si>
+    <t>33f45fc4a6d214df</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.f07b313808^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT2</t>
@@ -525,13 +525,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:21+02:00</t>
-  </si>
-  <si>
-    <t>1aff3e6ed976f043</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.14c195ecd6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:01+02:00</t>
+  </si>
+  <si>
+    <t>b9394cabbed5405b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.8b80104302^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT3</t>
@@ -542,13 +542,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:23+02:00</t>
-  </si>
-  <si>
-    <t>e5106ea969dd5ceb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.ece6331378^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:04+02:00</t>
+  </si>
+  <si>
+    <t>0c917ea707f73cf6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.633c246032^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT4</t>
@@ -559,13 +559,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:25+02:00</t>
-  </si>
-  <si>
-    <t>5c6a495c6f3ca8f1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.042ab781dc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:06+02:00</t>
+  </si>
+  <si>
+    <t>4d0a93903eed7653</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.3b896dd9c0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>CERT_VAC</t>
@@ -829,10 +829,10 @@
     </r>
   </si>
   <si>
-    <t>2023-08-01T10:28:28+02:00</t>
-  </si>
-  <si>
-    <t>e27a6d0be9833735</t>
+    <t>2023-08-02T17:57:08+02:00</t>
+  </si>
+  <si>
+    <t>b31c4b09b79c7bf5</t>
   </si>
   <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
@@ -847,10 +847,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:30+02:00</t>
-  </si>
-  <si>
-    <t>8c2378e902b22674</t>
+    <t>2023-08-02T17:57:10+02:00</t>
+  </si>
+  <si>
+    <t>93de67507603bf88</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_PSS_KO</t>
@@ -859,19 +859,19 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RAD_KO</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:31+02:00</t>
-  </si>
-  <si>
-    <t>480b79e03bc97752</t>
+    <t>2023-08-02T17:57:12+02:00</t>
+  </si>
+  <si>
+    <t>58bdc8b06157534c</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:33+02:00</t>
-  </si>
-  <si>
-    <t>4df18b4dbd84b2b8</t>
+    <t>2023-08-02T17:57:14+02:00</t>
+  </si>
+  <si>
+    <t>d2bd0b856922a7d7</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_CERT_VAC_KO</t>
@@ -921,13 +921,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:35+02:00</t>
-  </si>
-  <si>
-    <t>cd7ac4dee7638c20</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.b717bb6ff3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:15+02:00</t>
+  </si>
+  <si>
+    <t>c064e23e71bcb96c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.5c3e8cee5b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore di sintassi.</t>
@@ -950,13 +950,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:36+02:00</t>
-  </si>
-  <si>
-    <t>e8384b7d175c3d07</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.5af5f813f9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:17+02:00</t>
+  </si>
+  <si>
+    <t>f2edc05c12d3f408</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.556695aecb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore semantico.</t>
@@ -969,13 +969,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:38+02:00</t>
-  </si>
-  <si>
-    <t>29d16d404bb21a22</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.aac8cabc2a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:19+02:00</t>
+  </si>
+  <si>
+    <t>4552500208fe4dd4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.59bd966119^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT10_KO</t>
@@ -985,13 +985,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:40+02:00</t>
-  </si>
-  <si>
-    <t>6d5e18ce68c75748</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.16327a5e19^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:21+02:00</t>
+  </si>
+  <si>
+    <t>115f457311323ec8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.055609c9fd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT11_KO</t>
@@ -1001,13 +1001,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:42+02:00</t>
-  </si>
-  <si>
-    <t>1ce216074c6de10f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.b1ec81f117^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:22+02:00</t>
+  </si>
+  <si>
+    <t>ff09d67ca1a77894</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a47cbcd60f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore vocabolario.</t>
@@ -1020,13 +1020,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:43+02:00</t>
-  </si>
-  <si>
-    <t>6a71ef808ce8f90f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.25eea5de88^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:24+02:00</t>
+  </si>
+  <si>
+    <t>85a2ee9df11f26c1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.0813f0bc14^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT13_KO</t>
@@ -1036,13 +1036,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:45+02:00</t>
-  </si>
-  <si>
-    <t>d8357d62d7ae290e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a685242cdb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:26+02:00</t>
+  </si>
+  <si>
+    <t>d6d5e0d2bf6a0777</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.59d7d0b187^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT14_KO</t>
@@ -1052,13 +1052,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:47+02:00</t>
-  </si>
-  <si>
-    <t>3fad2b9245b5d7f5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.fe60105a4f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:28+02:00</t>
+  </si>
+  <si>
+    <t>a26a1959397f4cb4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.db6cf16572^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT15_KO</t>
@@ -1068,13 +1068,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:48+02:00</t>
-  </si>
-  <si>
-    <t>00cb2ceabbaf4103</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.ea6d957273^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:30+02:00</t>
+  </si>
+  <si>
+    <t>ddcddbddead14ac5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.6a0d8f8107^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT16_KO</t>
@@ -1084,13 +1084,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:28:50+02:00</t>
-  </si>
-  <si>
-    <t>6838903e2f7669ee</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.d1c60af85e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:32+02:00</t>
+  </si>
+  <si>
+    <t>56526f9e125b526f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a8e8bfbd10^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT5_KO</t>
@@ -1101,13 +1101,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-01T10:28:53+02:00</t>
-  </si>
-  <si>
-    <t>138d1ac68f9f6f46</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.17b48d7403^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:33+02:00</t>
+  </si>
+  <si>
+    <t>1b8dc828ab66c68d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.c7e6da6eb1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT6_KO</t>
@@ -1126,13 +1126,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-01T10:28:54+02:00</t>
-  </si>
-  <si>
-    <t>4de002558a125590</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.7efa3a4841^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:35+02:00</t>
+  </si>
+  <si>
+    <t>6a856718fed85b9a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.9b3ead2105^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT8_KO</t>
@@ -1143,13 +1143,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-01T10:28:56+02:00</t>
-  </si>
-  <si>
-    <t>7ca7dd23df5b7cdb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.22ef0ca0f8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:38+02:00</t>
+  </si>
+  <si>
+    <t>30673ad7e7d6d1ca</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.9f0019ccec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT9_KO</t>
@@ -1160,13 +1160,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-01T10:28:58+02:00</t>
-  </si>
-  <si>
-    <t>1271a4ecb4dc3923</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.abecbb3410^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:39+02:00</t>
+  </si>
+  <si>
+    <t>1a3afb4718684b58</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.20f576876e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT10_KO</t>
@@ -1177,13 +1177,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-01T10:29:00+02:00</t>
-  </si>
-  <si>
-    <t>22f9244e21e23a83</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.de0c810402^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:41+02:00</t>
+  </si>
+  <si>
+    <t>fe0c03667538cd8b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.593c3c53ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT11_KO</t>
@@ -1194,13 +1194,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-01T10:29:01+02:00</t>
-  </si>
-  <si>
-    <t>637dea875851bb2d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.1a93219b79^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:43+02:00</t>
+  </si>
+  <si>
+    <t>ee380a4204c2770a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.d58868dea1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT12_KO</t>
@@ -1211,13 +1211,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-01T10:29:03+02:00</t>
-  </si>
-  <si>
-    <t>c4f21b7ede1e2785</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.18901e338d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:45+02:00</t>
+  </si>
+  <si>
+    <t>5369831207315ea5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.5db705c7ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT13_KO</t>
@@ -1228,13 +1228,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-01T10:29:05+02:00</t>
-  </si>
-  <si>
-    <t>3cab6b134c26fce5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.b21ffd3ec6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:46+02:00</t>
+  </si>
+  <si>
+    <t>16adfb877fb04483</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.0e2af359c3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT14_KO</t>
@@ -1245,13 +1245,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-01T10:29:07+02:00</t>
-  </si>
-  <si>
-    <t>2574b04fd8f747e8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.4757c48409^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:48+02:00</t>
+  </si>
+  <si>
+    <t>b95b3fb7ba667523</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.5727a3eda4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT15_KO</t>
@@ -1262,13 +1262,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-01T10:29:08+02:00</t>
-  </si>
-  <si>
-    <t>d4149a3384cb00bc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.219f603715^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:50+02:00</t>
+  </si>
+  <si>
+    <t>bfece030bb7c6fe7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.d19f6f038f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT16_KO</t>
@@ -1279,13 +1279,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-01T10:29:10+02:00</t>
-  </si>
-  <si>
-    <t>7b6f05951091bee9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.3cf82249be^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:52+02:00</t>
+  </si>
+  <si>
+    <t>a0be71d9a15c35cf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.986dfd36d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT5_KO</t>
@@ -1296,13 +1296,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:12+02:00</t>
-  </si>
-  <si>
-    <t>ed9ca477999594cb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.f8b65d1e03^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:53+02:00</t>
+  </si>
+  <si>
+    <t>208bbd41f54af9a5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.181e354485^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT6_KO</t>
@@ -1320,13 +1320,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:14+02:00</t>
-  </si>
-  <si>
-    <t>c1de74cf22f1c661</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.a49c268729^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:55+02:00</t>
+  </si>
+  <si>
+    <t>0a37dc49de2f8fb8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.289aac7f51^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT8_KO</t>
@@ -1336,13 +1336,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:15+02:00</t>
-  </si>
-  <si>
-    <t>4ad9d8a874697985</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.43b957d261^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:57+02:00</t>
+  </si>
+  <si>
+    <t>5335cfa03ff63292</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.42fe72bdbf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT9_KO</t>
@@ -1353,13 +1353,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:17+02:00</t>
-  </si>
-  <si>
-    <t>6c4e178b44ba36bb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.11f19d91b7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:57:59+02:00</t>
+  </si>
+  <si>
+    <t>7bc83a069a48318f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.06bb4954b4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT10_KO</t>
@@ -1370,13 +1370,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:20+02:00</t>
-  </si>
-  <si>
-    <t>a3e6ee490433b544</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.c5be65ee68^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:00+02:00</t>
+  </si>
+  <si>
+    <t>ca9399807fd104e4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.16eeec0621^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT11_KO</t>
@@ -1387,13 +1387,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:23+02:00</t>
-  </si>
-  <si>
-    <t>53c9567b8b99f97d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.bdb6058ebb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:02+02:00</t>
+  </si>
+  <si>
+    <t>fb84e2ea3c9a5ec4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.f55c7b8f6f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT12_KO</t>
@@ -1404,13 +1404,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:25+02:00</t>
-  </si>
-  <si>
-    <t>a922131b0e5ab8af</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.8dc81e450c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:04+02:00</t>
+  </si>
+  <si>
+    <t>b091e214eba9ad35</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.2aa8226b6e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT13_KO</t>
@@ -1420,13 +1420,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:26+02:00</t>
-  </si>
-  <si>
-    <t>61b304b623b12926</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.625f42cee1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:06+02:00</t>
+  </si>
+  <si>
+    <t>75ab022118a943ac</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d8cd9aa509^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT14_KO</t>
@@ -1436,13 +1436,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:28+02:00</t>
-  </si>
-  <si>
-    <t>191a7b22835f40d4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d0bf150bc5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:07+02:00</t>
+  </si>
+  <si>
+    <t>26777e55fe3e566b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d66109a612^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT15_KO</t>
@@ -1453,13 +1453,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:30+02:00</t>
-  </si>
-  <si>
-    <t>fb81e0716d0bc91c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.1d2798f9ac^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:10+02:00</t>
+  </si>
+  <si>
+    <t>41842e9fc10c0760</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.c83de000cb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT16_KO</t>
@@ -1470,13 +1470,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:31+02:00</t>
-  </si>
-  <si>
-    <t>01cc9343e9b5e342</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d9bf75e321^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:12+02:00</t>
+  </si>
+  <si>
+    <t>863558cf098a0ec3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.23433fa939^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT17_KO</t>
@@ -1487,13 +1487,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:33+02:00</t>
-  </si>
-  <si>
-    <t>1115d74bfe8fcd03</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.4e420a955c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:14+02:00</t>
+  </si>
+  <si>
+    <t>4df24a3ab6b56d07</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.4987e8dd27^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT18_KO</t>
@@ -1504,13 +1504,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:35+02:00</t>
-  </si>
-  <si>
-    <t>8f99ddc2247ccdba</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.e732cde4fe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:16+02:00</t>
+  </si>
+  <si>
+    <t>8c2aee5458cb57e1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.5e26462cf7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT19_KO</t>
@@ -1520,13 +1520,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:37+02:00</t>
-  </si>
-  <si>
-    <t>5f8aefced4f7729f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b7daef18e4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:17+02:00</t>
+  </si>
+  <si>
+    <t>a507200067e82524</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.15e9cee836^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT20_KO</t>
@@ -1536,13 +1536,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:38+02:00</t>
-  </si>
-  <si>
-    <t>53eee0b884f743a6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.be9f0ca65d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:19+02:00</t>
+  </si>
+  <si>
+    <t>07747d9d4c5ef757</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.273999ee41^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT21_KO</t>
@@ -1553,13 +1553,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:40+02:00</t>
-  </si>
-  <si>
-    <t>247396bb6d837196</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.f6379101a7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:21+02:00</t>
+  </si>
+  <si>
+    <t>afaac2f5a4a7f8f4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.a61e583437^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT22_KO</t>
@@ -1570,13 +1570,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:42+02:00</t>
-  </si>
-  <si>
-    <t>09ac537b60b5d26c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d9ce353b3c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:23+02:00</t>
+  </si>
+  <si>
+    <t>ad76b4d03cfa4ecc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.1c6c129ca7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT23_KO</t>
@@ -1587,13 +1587,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:44+02:00</t>
-  </si>
-  <si>
-    <t>41886a7e0856d0c0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.919797dedc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:24+02:00</t>
+  </si>
+  <si>
+    <t>241accf72ee6057c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b8b079bd0e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT5_KO</t>
@@ -2007,13 +2007,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-01T10:30:19+02:00</t>
-  </si>
-  <si>
-    <t>62ea4a7a9422bbdf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.ada109782a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:58+02:00</t>
+  </si>
+  <si>
+    <t>5b6071125ec0679a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.1ea252a196^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT2</t>
@@ -2025,13 +2025,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-01T10:30:21+02:00</t>
-  </si>
-  <si>
-    <t>25f1a33327d7e78d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.54a9fa09da^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:59:00+02:00</t>
+  </si>
+  <si>
+    <t>af930d43e1e4968f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c60bbf120c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT3</t>
@@ -2043,13 +2043,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-01T10:30:23+02:00</t>
-  </si>
-  <si>
-    <t>47ac5543452da7d8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.51e1d0f757^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:59:02+02:00</t>
+  </si>
+  <si>
+    <t>16cd1bdb945814e8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.2857070f35^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT4</t>
@@ -2061,13 +2061,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-01T10:30:24+02:00</t>
-  </si>
-  <si>
-    <t>8d4d065f4633a742</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.76e63fd26f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:59:04+02:00</t>
+  </si>
+  <si>
+    <t>66b46f9a7f1c30e0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.b8b1dc4788^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT5_KO</t>
@@ -2077,13 +2077,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:47+02:00</t>
-  </si>
-  <si>
-    <t>987b5738582612a8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.71f08f3766^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:26+02:00</t>
+  </si>
+  <si>
+    <t>42ed6e0e1e9443be</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.687857d670^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT6_KO</t>
@@ -2102,13 +2102,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:48+02:00</t>
-  </si>
-  <si>
-    <t>22157bccac582823</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c48e622365^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:28+02:00</t>
+  </si>
+  <si>
+    <t>a05aa83ce6c8bbbb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.d21787a681^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT8_KO</t>
@@ -2119,13 +2119,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:50+02:00</t>
-  </si>
-  <si>
-    <t>a45f643cde42d2dd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.7fa634ce0d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:29+02:00</t>
+  </si>
+  <si>
+    <t>84c3273212a404cc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.ed6a5b0589^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT9_KO</t>
@@ -2136,13 +2136,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:52+02:00</t>
-  </si>
-  <si>
-    <t>465870736d4d2a43</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.520c34060d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:32+02:00</t>
+  </si>
+  <si>
+    <t>514686b088af1c69</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.ed51f403a0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT10_KO</t>
@@ -2153,13 +2153,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:54+02:00</t>
-  </si>
-  <si>
-    <t>6bdbedc28ac33a79</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.9ff72faf16^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:34+02:00</t>
+  </si>
+  <si>
+    <t>561df35a74756d43</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.518acbc4cb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT11_KO</t>
@@ -2170,13 +2170,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:56+02:00</t>
-  </si>
-  <si>
-    <t>f4f1106902951eec</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.189f5c1b5b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:35+02:00</t>
+  </si>
+  <si>
+    <t>14b964d574cbcc9e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.789775c3f1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT12_KO</t>
@@ -2187,13 +2187,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:29:58+02:00</t>
-  </si>
-  <si>
-    <t>3c71011db7cfd822</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.210274ebd7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:37+02:00</t>
+  </si>
+  <si>
+    <t>c90a5ec4ffe8e901</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5cb23ca923^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT13_KO</t>
@@ -2203,13 +2203,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:30:00+02:00</t>
-  </si>
-  <si>
-    <t>0230b517a152dde7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.acd149c843^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:39+02:00</t>
+  </si>
+  <si>
+    <t>9d7a89c6f271a0c2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.227ddd8d66^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT14_KO</t>
@@ -2219,13 +2219,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:30:02+02:00</t>
-  </si>
-  <si>
-    <t>691468ec6cea676a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.ead61386a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:41+02:00</t>
+  </si>
+  <si>
+    <t>1c704d9b345357bc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.604734fa47^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT15_KO</t>
@@ -2236,13 +2236,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:30:03+02:00</t>
-  </si>
-  <si>
-    <t>3ce76b04949d4060</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.b350af67dc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:42+02:00</t>
+  </si>
+  <si>
+    <t>129406cd8882f40c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.61df45a12b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT16_KO</t>
@@ -2253,13 +2253,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:30:05+02:00</t>
-  </si>
-  <si>
-    <t>95f81e89f98a67e5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.878a5b45ec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:44+02:00</t>
+  </si>
+  <si>
+    <t>02ebb1bb3d74c8f6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.599358719b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT17_KO</t>
@@ -2270,13 +2270,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:30:07+02:00</t>
-  </si>
-  <si>
-    <t>7f5093576c17a756</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c3a8090636^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:46+02:00</t>
+  </si>
+  <si>
+    <t>0f81546819e32ba6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.7e5c5b5bce^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT18_KO</t>
@@ -2287,13 +2287,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:30:09+02:00</t>
-  </si>
-  <si>
-    <t>9b3fa85484e1e123</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.6c4e80e4bb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:48+02:00</t>
+  </si>
+  <si>
+    <t>5a636ba6b0f204e3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.ec770971a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT19_KO</t>
@@ -2304,13 +2304,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:30:10+02:00</t>
-  </si>
-  <si>
-    <t>34466c58255d6bb8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.307416dfe4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:49+02:00</t>
+  </si>
+  <si>
+    <t>8c46a5ade198aff4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.36b49ef7e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT20_KO</t>
@@ -2321,13 +2321,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:30:12+02:00</t>
-  </si>
-  <si>
-    <t>e48ccad7ba8f6858</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.60b2f0667f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:51+02:00</t>
+  </si>
+  <si>
+    <t>ed05bc26fee47d97</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.38000c4401^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT21_KO</t>
@@ -2338,13 +2338,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:30:14+02:00</t>
-  </si>
-  <si>
-    <t>1084ae4ad0c245d4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.69c6cbc062^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:53+02:00</t>
+  </si>
+  <si>
+    <t>daa28e032f7b6c95</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.b90d411753^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT22_KO</t>
@@ -2355,13 +2355,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:30:15+02:00</t>
-  </si>
-  <si>
-    <t>81e3102ebfaaa569</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.0fdcec6e2c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:55+02:00</t>
+  </si>
+  <si>
+    <t>9da30ca5d7fe3117</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.188679481b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT23_KO</t>
@@ -2372,13 +2372,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:30:17+02:00</t>
-  </si>
-  <si>
-    <t>6acb89eb6a45e4a3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.9a54eb92ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:58:56+02:00</t>
+  </si>
+  <si>
+    <t>d8f60ae069419e8b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.987e775898^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_PSS_CT1</t>
@@ -2560,13 +2560,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-01T10:30:26+02:00</t>
-  </si>
-  <si>
-    <t>f400e707483e8a68</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.b74f5df021^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:59:05+02:00</t>
+  </si>
+  <si>
+    <t>f39a50fc1890d758</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.d892ce756c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>PUBBLICAZIONE_CREAZIONE</t>
@@ -4560,13 +4560,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-01T10:30:28+02:00</t>
-  </si>
-  <si>
-    <t>0ce9d2ee139ba717</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.535636202b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:59:07+02:00</t>
+  </si>
+  <si>
+    <t>a76abb028527122a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a8f09a2206^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT0</t>
@@ -4577,13 +4577,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:30:30+02:00</t>
-  </si>
-  <si>
-    <t>5d31158c1d85e6f9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.2e41aeb0f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:59:09+02:00</t>
+  </si>
+  <si>
+    <t>8048fe8c2bc50ac9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.46e92dcc10^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT0</t>
@@ -4594,13 +4594,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-01T10:30:31+02:00</t>
-  </si>
-  <si>
-    <t>6ed50931aaa3d5fb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.9484a37ef1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:59:11+02:00</t>
+  </si>
+  <si>
+    <t>3fb029f33990bff4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.f9961af97f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT0</t>
@@ -4636,13 +4636,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-01T10:30:33+02:00</t>
-  </si>
-  <si>
-    <t>4bc419e7e1d6649c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.370cb79d81^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:59:13+02:00</t>
+  </si>
+  <si>
+    <t>04d1382bd530100d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.4b1f94c4cf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_PSS_CT0</t>
@@ -4663,13 +4663,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-01T10:30:35+02:00</t>
-  </si>
-  <si>
-    <t>660b8e4d68a02900</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.262ca5073c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-02T17:59:14+02:00</t>
+  </si>
+  <si>
+    <t>32a58c44dfe13150</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.39e3e0a4e3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ID TEST CASE OK</t>
@@ -9412,7 +9412,9 @@
         <v>56</v>
       </c>
       <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
+      <c r="L43" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M43" s="25" t="s">
         <v>124</v>
       </c>
@@ -9466,7 +9468,9 @@
         <v>56</v>
       </c>
       <c r="K44" s="25"/>
-      <c r="L44" s="25"/>
+      <c r="L44" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M44" s="25" t="s">
         <v>124</v>
       </c>
@@ -9558,7 +9562,9 @@
         <v>56</v>
       </c>
       <c r="K46" s="25"/>
-      <c r="L46" s="25"/>
+      <c r="L46" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M46" s="25" t="s">
         <v>124</v>
       </c>
@@ -9612,7 +9618,9 @@
         <v>56</v>
       </c>
       <c r="K47" s="25"/>
-      <c r="L47" s="25"/>
+      <c r="L47" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M47" s="25" t="s">
         <v>124</v>
       </c>
@@ -10132,7 +10140,9 @@
         <v>56</v>
       </c>
       <c r="K59" s="25"/>
-      <c r="L59" s="25"/>
+      <c r="L59" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M59" s="25" t="s">
         <v>124</v>
       </c>
@@ -10224,7 +10234,9 @@
         <v>56</v>
       </c>
       <c r="K61" s="25"/>
-      <c r="L61" s="25"/>
+      <c r="L61" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M61" s="25" t="s">
         <v>124</v>
       </c>
@@ -10278,7 +10290,9 @@
         <v>56</v>
       </c>
       <c r="K62" s="25"/>
-      <c r="L62" s="25"/>
+      <c r="L62" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M62" s="25" t="s">
         <v>124</v>
       </c>
@@ -10332,7 +10346,9 @@
         <v>56</v>
       </c>
       <c r="K63" s="25"/>
-      <c r="L63" s="25"/>
+      <c r="L63" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M63" s="25" t="s">
         <v>124</v>
       </c>
@@ -10386,7 +10402,9 @@
         <v>56</v>
       </c>
       <c r="K64" s="25"/>
-      <c r="L64" s="25"/>
+      <c r="L64" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M64" s="25" t="s">
         <v>124</v>
       </c>
@@ -10440,7 +10458,9 @@
         <v>56</v>
       </c>
       <c r="K65" s="25"/>
-      <c r="L65" s="25"/>
+      <c r="L65" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M65" s="25" t="s">
         <v>124</v>
       </c>
@@ -10494,7 +10514,9 @@
         <v>56</v>
       </c>
       <c r="K66" s="25"/>
-      <c r="L66" s="25"/>
+      <c r="L66" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M66" s="25" t="s">
         <v>124</v>
       </c>
@@ -10548,7 +10570,9 @@
         <v>56</v>
       </c>
       <c r="K67" s="25"/>
-      <c r="L67" s="25"/>
+      <c r="L67" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M67" s="25" t="s">
         <v>124</v>
       </c>
@@ -10602,7 +10626,9 @@
         <v>56</v>
       </c>
       <c r="K68" s="25"/>
-      <c r="L68" s="25"/>
+      <c r="L68" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M68" s="25" t="s">
         <v>124</v>
       </c>
@@ -10656,7 +10682,9 @@
         <v>56</v>
       </c>
       <c r="K69" s="25"/>
-      <c r="L69" s="25"/>
+      <c r="L69" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M69" s="25" t="s">
         <v>124</v>
       </c>
@@ -10710,7 +10738,9 @@
         <v>56</v>
       </c>
       <c r="K70" s="25"/>
-      <c r="L70" s="25"/>
+      <c r="L70" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M70" s="25" t="s">
         <v>124</v>
       </c>
@@ -10802,7 +10832,9 @@
         <v>56</v>
       </c>
       <c r="K72" s="25"/>
-      <c r="L72" s="25"/>
+      <c r="L72" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M72" s="25" t="s">
         <v>124</v>
       </c>
@@ -10856,7 +10888,9 @@
         <v>56</v>
       </c>
       <c r="K73" s="25"/>
-      <c r="L73" s="25"/>
+      <c r="L73" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M73" s="25" t="s">
         <v>124</v>
       </c>
@@ -10910,7 +10944,9 @@
         <v>56</v>
       </c>
       <c r="K74" s="25"/>
-      <c r="L74" s="25"/>
+      <c r="L74" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M74" s="25" t="s">
         <v>124</v>
       </c>
@@ -10964,7 +11000,9 @@
         <v>56</v>
       </c>
       <c r="K75" s="25"/>
-      <c r="L75" s="25"/>
+      <c r="L75" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M75" s="25" t="s">
         <v>124</v>
       </c>
@@ -11018,7 +11056,9 @@
         <v>56</v>
       </c>
       <c r="K76" s="25"/>
-      <c r="L76" s="25"/>
+      <c r="L76" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M76" s="25" t="s">
         <v>124</v>
       </c>
@@ -11072,7 +11112,9 @@
         <v>56</v>
       </c>
       <c r="K77" s="25"/>
-      <c r="L77" s="25"/>
+      <c r="L77" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M77" s="25" t="s">
         <v>124</v>
       </c>
@@ -11126,7 +11168,9 @@
         <v>56</v>
       </c>
       <c r="K78" s="25"/>
-      <c r="L78" s="25"/>
+      <c r="L78" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M78" s="25" t="s">
         <v>124</v>
       </c>
@@ -11180,7 +11224,9 @@
         <v>56</v>
       </c>
       <c r="K79" s="25"/>
-      <c r="L79" s="25"/>
+      <c r="L79" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M79" s="25" t="s">
         <v>124</v>
       </c>
@@ -11234,7 +11280,9 @@
         <v>56</v>
       </c>
       <c r="K80" s="25"/>
-      <c r="L80" s="25"/>
+      <c r="L80" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M80" s="25" t="s">
         <v>124</v>
       </c>
@@ -11288,7 +11336,9 @@
         <v>56</v>
       </c>
       <c r="K81" s="25"/>
-      <c r="L81" s="25"/>
+      <c r="L81" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M81" s="25" t="s">
         <v>124</v>
       </c>
@@ -11342,7 +11392,9 @@
         <v>56</v>
       </c>
       <c r="K82" s="25"/>
-      <c r="L82" s="25"/>
+      <c r="L82" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M82" s="25" t="s">
         <v>124</v>
       </c>
@@ -11434,7 +11486,9 @@
         <v>56</v>
       </c>
       <c r="K84" s="25"/>
-      <c r="L84" s="25"/>
+      <c r="L84" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M84" s="25" t="s">
         <v>124</v>
       </c>
@@ -11488,7 +11542,9 @@
         <v>56</v>
       </c>
       <c r="K85" s="25"/>
-      <c r="L85" s="25"/>
+      <c r="L85" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M85" s="25" t="s">
         <v>124</v>
       </c>
@@ -11542,7 +11598,9 @@
         <v>56</v>
       </c>
       <c r="K86" s="25"/>
-      <c r="L86" s="25"/>
+      <c r="L86" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M86" s="25" t="s">
         <v>124</v>
       </c>
@@ -11596,7 +11654,9 @@
         <v>56</v>
       </c>
       <c r="K87" s="25"/>
-      <c r="L87" s="25"/>
+      <c r="L87" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M87" s="25" t="s">
         <v>124</v>
       </c>
@@ -11650,7 +11710,9 @@
         <v>56</v>
       </c>
       <c r="K88" s="25"/>
-      <c r="L88" s="25"/>
+      <c r="L88" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M88" s="25" t="s">
         <v>124</v>
       </c>
@@ -11704,7 +11766,9 @@
         <v>56</v>
       </c>
       <c r="K89" s="25"/>
-      <c r="L89" s="25"/>
+      <c r="L89" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M89" s="25" t="s">
         <v>124</v>
       </c>
@@ -11758,7 +11822,9 @@
         <v>56</v>
       </c>
       <c r="K90" s="25"/>
-      <c r="L90" s="25"/>
+      <c r="L90" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M90" s="25" t="s">
         <v>124</v>
       </c>
@@ -11812,7 +11878,9 @@
         <v>56</v>
       </c>
       <c r="K91" s="25"/>
-      <c r="L91" s="25"/>
+      <c r="L91" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M91" s="25" t="s">
         <v>124</v>
       </c>
@@ -11866,7 +11934,9 @@
         <v>56</v>
       </c>
       <c r="K92" s="25"/>
-      <c r="L92" s="25"/>
+      <c r="L92" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M92" s="25" t="s">
         <v>124</v>
       </c>
@@ -11920,7 +11990,9 @@
         <v>56</v>
       </c>
       <c r="K93" s="25"/>
-      <c r="L93" s="25"/>
+      <c r="L93" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M93" s="25" t="s">
         <v>124</v>
       </c>
@@ -11974,7 +12046,9 @@
         <v>56</v>
       </c>
       <c r="K94" s="25"/>
-      <c r="L94" s="25"/>
+      <c r="L94" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M94" s="25" t="s">
         <v>124</v>
       </c>
@@ -12028,7 +12102,9 @@
         <v>56</v>
       </c>
       <c r="K95" s="25"/>
-      <c r="L95" s="25"/>
+      <c r="L95" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M95" s="25" t="s">
         <v>124</v>
       </c>
@@ -12082,7 +12158,9 @@
         <v>56</v>
       </c>
       <c r="K96" s="25"/>
-      <c r="L96" s="25"/>
+      <c r="L96" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M96" s="25" t="s">
         <v>124</v>
       </c>
@@ -12136,7 +12214,9 @@
         <v>56</v>
       </c>
       <c r="K97" s="25"/>
-      <c r="L97" s="25"/>
+      <c r="L97" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M97" s="25" t="s">
         <v>124</v>
       </c>
@@ -12190,7 +12270,9 @@
         <v>56</v>
       </c>
       <c r="K98" s="25"/>
-      <c r="L98" s="25"/>
+      <c r="L98" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M98" s="25" t="s">
         <v>124</v>
       </c>
@@ -12244,7 +12326,9 @@
         <v>56</v>
       </c>
       <c r="K99" s="25"/>
-      <c r="L99" s="25"/>
+      <c r="L99" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M99" s="25" t="s">
         <v>124</v>
       </c>
@@ -12298,7 +12382,9 @@
         <v>56</v>
       </c>
       <c r="K100" s="25"/>
-      <c r="L100" s="25"/>
+      <c r="L100" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M100" s="25" t="s">
         <v>124</v>
       </c>
@@ -14550,7 +14636,9 @@
         <v>56</v>
       </c>
       <c r="K158" s="25"/>
-      <c r="L158" s="25"/>
+      <c r="L158" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M158" s="25" t="s">
         <v>124</v>
       </c>
@@ -14642,7 +14730,9 @@
         <v>56</v>
       </c>
       <c r="K160" s="25"/>
-      <c r="L160" s="25"/>
+      <c r="L160" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M160" s="25" t="s">
         <v>124</v>
       </c>
@@ -14696,7 +14786,9 @@
         <v>56</v>
       </c>
       <c r="K161" s="25"/>
-      <c r="L161" s="25"/>
+      <c r="L161" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M161" s="25" t="s">
         <v>124</v>
       </c>
@@ -14750,7 +14842,9 @@
         <v>56</v>
       </c>
       <c r="K162" s="25"/>
-      <c r="L162" s="25"/>
+      <c r="L162" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M162" s="25" t="s">
         <v>124</v>
       </c>
@@ -14804,7 +14898,9 @@
         <v>56</v>
       </c>
       <c r="K163" s="25"/>
-      <c r="L163" s="25"/>
+      <c r="L163" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M163" s="25" t="s">
         <v>124</v>
       </c>
@@ -14858,7 +14954,9 @@
         <v>56</v>
       </c>
       <c r="K164" s="25"/>
-      <c r="L164" s="25"/>
+      <c r="L164" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M164" s="25" t="s">
         <v>124</v>
       </c>
@@ -14912,7 +15010,9 @@
         <v>56</v>
       </c>
       <c r="K165" s="25"/>
-      <c r="L165" s="25"/>
+      <c r="L165" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M165" s="25" t="s">
         <v>124</v>
       </c>
@@ -14966,7 +15066,9 @@
         <v>56</v>
       </c>
       <c r="K166" s="25"/>
-      <c r="L166" s="25"/>
+      <c r="L166" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M166" s="25" t="s">
         <v>124</v>
       </c>
@@ -15020,7 +15122,9 @@
         <v>56</v>
       </c>
       <c r="K167" s="25"/>
-      <c r="L167" s="25"/>
+      <c r="L167" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M167" s="25" t="s">
         <v>124</v>
       </c>
@@ -15074,7 +15178,9 @@
         <v>56</v>
       </c>
       <c r="K168" s="25"/>
-      <c r="L168" s="25"/>
+      <c r="L168" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M168" s="25" t="s">
         <v>124</v>
       </c>
@@ -15128,7 +15234,9 @@
         <v>56</v>
       </c>
       <c r="K169" s="25"/>
-      <c r="L169" s="25"/>
+      <c r="L169" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M169" s="25" t="s">
         <v>124</v>
       </c>
@@ -15182,7 +15290,9 @@
         <v>56</v>
       </c>
       <c r="K170" s="25"/>
-      <c r="L170" s="25"/>
+      <c r="L170" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M170" s="25" t="s">
         <v>124</v>
       </c>
@@ -15236,7 +15346,9 @@
         <v>56</v>
       </c>
       <c r="K171" s="25"/>
-      <c r="L171" s="25"/>
+      <c r="L171" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M171" s="25" t="s">
         <v>124</v>
       </c>
@@ -15290,7 +15402,9 @@
         <v>56</v>
       </c>
       <c r="K172" s="25"/>
-      <c r="L172" s="25"/>
+      <c r="L172" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M172" s="25" t="s">
         <v>124</v>
       </c>
@@ -15344,7 +15458,9 @@
         <v>56</v>
       </c>
       <c r="K173" s="25"/>
-      <c r="L173" s="25"/>
+      <c r="L173" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M173" s="25" t="s">
         <v>124</v>
       </c>
@@ -15398,7 +15514,9 @@
         <v>56</v>
       </c>
       <c r="K174" s="25"/>
-      <c r="L174" s="25"/>
+      <c r="L174" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M174" s="25" t="s">
         <v>124</v>
       </c>
@@ -15452,7 +15570,9 @@
         <v>56</v>
       </c>
       <c r="K175" s="25"/>
-      <c r="L175" s="25"/>
+      <c r="L175" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M175" s="25" t="s">
         <v>124</v>
       </c>
@@ -15506,7 +15626,9 @@
         <v>56</v>
       </c>
       <c r="K176" s="25"/>
-      <c r="L176" s="25"/>
+      <c r="L176" s="25" t="s">
+        <v>124</v>
+      </c>
       <c r="M176" s="25" t="s">
         <v>124</v>
       </c>

</xml_diff>

<commit_message>
Correzioni errori indicati da precedente mancanza accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SPEITSRL/SPE.IT s.r.l/FSE INI Adapter/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111SPEITSRL/SPE.IT s.r.l/FSE INI Adapter/1.0/report-checklist.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1097">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -333,16 +333,16 @@
 </t>
   </si>
   <si>
-    <t>02/08/2023</t>
-  </si>
-  <si>
-    <t>2023-08-02T17:56:28+02:00</t>
-  </si>
-  <si>
-    <t>a61b9d5076a638d0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.5a6f3098d9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>09/08/2023</t>
+  </si>
+  <si>
+    <t>2023-08-09T17:50:58+02:00</t>
+  </si>
+  <si>
+    <t>ff990bea1a322f0c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.e34a1fab6a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -363,13 +363,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-02T17:56:45+02:00</t>
-  </si>
-  <si>
-    <t>ce55c4b3da3067f6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.f5df58baa1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:01+02:00</t>
+  </si>
+  <si>
+    <t>233492747b5e55c0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.3eb3ee7101^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT3</t>
@@ -381,13 +381,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-02T17:56:47+02:00</t>
-  </si>
-  <si>
-    <t>5865ccb7d18d14cd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.8a2d98fa4c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:03+02:00</t>
+  </si>
+  <si>
+    <t>b658e07d4ec49f3c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.adeb01a5aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT4</t>
@@ -399,13 +399,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-02T17:56:48+02:00</t>
-  </si>
-  <si>
-    <t>5bc6e2450dff7da6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.6f4ddae6f4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:05+02:00</t>
+  </si>
+  <si>
+    <t>95583b99165f575f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.4d43c16813^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT5</t>
@@ -417,13 +417,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-02T17:56:50+02:00</t>
-  </si>
-  <si>
-    <t>7b373dc685e91191</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.8827466ab8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:07+02:00</t>
+  </si>
+  <si>
+    <t>229dc8493b43b728</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.7f5d619b19^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>LDO</t>
@@ -437,13 +437,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:56:52+02:00</t>
-  </si>
-  <si>
-    <t>09d3642d20f2fadc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.e15b237bd2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:09+02:00</t>
+  </si>
+  <si>
+    <t>66bb6eec1c6d641f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.98f7e0cec0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT2</t>
@@ -454,13 +454,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:56:54+02:00</t>
-  </si>
-  <si>
-    <t>9043852718eac292</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.e35aa06c53^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:11+02:00</t>
+  </si>
+  <si>
+    <t>1297c717f82d1d22</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.5f5012873d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT3</t>
@@ -471,13 +471,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:56:56+02:00</t>
-  </si>
-  <si>
-    <t>f606b8d380a7fc6e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.94dd5c9716^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:13+02:00</t>
+  </si>
+  <si>
+    <t>e15879cac42b117b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.3ea6da98df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT4</t>
@@ -488,13 +488,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:56:58+02:00</t>
-  </si>
-  <si>
-    <t>0e88eca633171ebb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.ab3c47553a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:15+02:00</t>
+  </si>
+  <si>
+    <t>448fe0844a6ef5f2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.b971e897de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>RAD</t>
@@ -508,13 +508,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:56:59+02:00</t>
-  </si>
-  <si>
-    <t>33f45fc4a6d214df</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.f07b313808^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:18+02:00</t>
+  </si>
+  <si>
+    <t>184a60cc80e70db1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.8c13dc732a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT2</t>
@@ -525,13 +525,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:01+02:00</t>
-  </si>
-  <si>
-    <t>b9394cabbed5405b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.8b80104302^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:20+02:00</t>
+  </si>
+  <si>
+    <t>43d0be61ed35e02a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.a09163b23b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT3</t>
@@ -542,13 +542,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:04+02:00</t>
-  </si>
-  <si>
-    <t>0c917ea707f73cf6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.633c246032^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:22+02:00</t>
+  </si>
+  <si>
+    <t>fcf858dcf077f452</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.bf6230c4df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT4</t>
@@ -559,13 +559,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:06+02:00</t>
-  </si>
-  <si>
-    <t>4d0a93903eed7653</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.3b896dd9c0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:24+02:00</t>
+  </si>
+  <si>
+    <t>5dab3157b255f84a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.8dc02c8ceb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>CERT_VAC</t>
@@ -829,10 +829,10 @@
     </r>
   </si>
   <si>
-    <t>2023-08-02T17:57:08+02:00</t>
-  </si>
-  <si>
-    <t>b31c4b09b79c7bf5</t>
+    <t>2023-08-09T17:51:26+02:00</t>
+  </si>
+  <si>
+    <t>3f99a0b7f2a193e6</t>
   </si>
   <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
@@ -847,10 +847,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:10+02:00</t>
-  </si>
-  <si>
-    <t>93de67507603bf88</t>
+    <t>2023-08-09T17:51:29+02:00</t>
+  </si>
+  <si>
+    <t>08761ab3bf9e3ad2</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_PSS_KO</t>
@@ -859,19 +859,19 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RAD_KO</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:12+02:00</t>
-  </si>
-  <si>
-    <t>58bdc8b06157534c</t>
+    <t>2023-08-09T17:51:31+02:00</t>
+  </si>
+  <si>
+    <t>db0b03df7758bd2a</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:14+02:00</t>
-  </si>
-  <si>
-    <t>d2bd0b856922a7d7</t>
+    <t>2023-08-09T17:51:33+02:00</t>
+  </si>
+  <si>
+    <t>f926021cfda0e2eb</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_CERT_VAC_KO</t>
@@ -921,13 +921,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:15+02:00</t>
-  </si>
-  <si>
-    <t>c064e23e71bcb96c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.5c3e8cee5b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:35+02:00</t>
+  </si>
+  <si>
+    <t>013fa11e746877ec</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.1222b8109c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore di sintassi.</t>
@@ -950,13 +950,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:17+02:00</t>
-  </si>
-  <si>
-    <t>f2edc05c12d3f408</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.556695aecb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:37+02:00</t>
+  </si>
+  <si>
+    <t>4c2f604cafcd775f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a21a1909a2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore semantico.</t>
@@ -969,13 +969,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:19+02:00</t>
-  </si>
-  <si>
-    <t>4552500208fe4dd4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.59bd966119^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:39+02:00</t>
+  </si>
+  <si>
+    <t>110c2c0cadafadb7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.7da2cae15d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT10_KO</t>
@@ -985,13 +985,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:21+02:00</t>
-  </si>
-  <si>
-    <t>115f457311323ec8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.055609c9fd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:41+02:00</t>
+  </si>
+  <si>
+    <t>9f4edf35f336735b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.f3b8431904^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT11_KO</t>
@@ -1001,13 +1001,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:22+02:00</t>
-  </si>
-  <si>
-    <t>ff09d67ca1a77894</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a47cbcd60f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:43+02:00</t>
+  </si>
+  <si>
+    <t>a70062f16f7023c4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.6c46179b61^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore vocabolario.</t>
@@ -1020,13 +1020,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:24+02:00</t>
-  </si>
-  <si>
-    <t>85a2ee9df11f26c1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.0813f0bc14^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:46+02:00</t>
+  </si>
+  <si>
+    <t>d3c639b368cc52db</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.8e661a1f50^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT13_KO</t>
@@ -1036,13 +1036,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:26+02:00</t>
-  </si>
-  <si>
-    <t>d6d5e0d2bf6a0777</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.59d7d0b187^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:48+02:00</t>
+  </si>
+  <si>
+    <t>08cae0e036da3356</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.d7ed938e18^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT14_KO</t>
@@ -1052,13 +1052,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:28+02:00</t>
-  </si>
-  <si>
-    <t>a26a1959397f4cb4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.db6cf16572^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:50+02:00</t>
+  </si>
+  <si>
+    <t>6dcddfe4a1e001bc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.00e8e03982^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT15_KO</t>
@@ -1068,13 +1068,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:30+02:00</t>
-  </si>
-  <si>
-    <t>ddcddbddead14ac5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.6a0d8f8107^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:52+02:00</t>
+  </si>
+  <si>
+    <t>f41fcc47453a7192</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.6f94ec95c5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT16_KO</t>
@@ -1084,13 +1084,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:32+02:00</t>
-  </si>
-  <si>
-    <t>56526f9e125b526f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a8e8bfbd10^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:54+02:00</t>
+  </si>
+  <si>
+    <t>662266052a49f579</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.b92cd78908^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT5_KO</t>
@@ -1101,13 +1101,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-02T17:57:33+02:00</t>
-  </si>
-  <si>
-    <t>1b8dc828ab66c68d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.c7e6da6eb1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:56+02:00</t>
+  </si>
+  <si>
+    <t>270048e2de5cccfd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.770c0a0afd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT6_KO</t>
@@ -1126,13 +1126,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-02T17:57:35+02:00</t>
-  </si>
-  <si>
-    <t>6a856718fed85b9a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.9b3ead2105^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:51:58+02:00</t>
+  </si>
+  <si>
+    <t>f279c095246a41ca</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.75e69533f6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT8_KO</t>
@@ -1143,13 +1143,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-02T17:57:38+02:00</t>
-  </si>
-  <si>
-    <t>30673ad7e7d6d1ca</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.9f0019ccec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:00+02:00</t>
+  </si>
+  <si>
+    <t>4172635a2cba6aab</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.b2cf82d636^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT9_KO</t>
@@ -1160,13 +1160,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-02T17:57:39+02:00</t>
-  </si>
-  <si>
-    <t>1a3afb4718684b58</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.20f576876e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:02+02:00</t>
+  </si>
+  <si>
+    <t>6b8896078ef38bb8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.770a11571b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT10_KO</t>
@@ -1177,13 +1177,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-02T17:57:41+02:00</t>
-  </si>
-  <si>
-    <t>fe0c03667538cd8b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.593c3c53ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:04+02:00</t>
+  </si>
+  <si>
+    <t>d5e5b5cd3fbf6900</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.fd13a223a4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT11_KO</t>
@@ -1194,13 +1194,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-02T17:57:43+02:00</t>
-  </si>
-  <si>
-    <t>ee380a4204c2770a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.d58868dea1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:06+02:00</t>
+  </si>
+  <si>
+    <t>e4174148d987259e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.5c196344e0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT12_KO</t>
@@ -1211,13 +1211,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-02T17:57:45+02:00</t>
-  </si>
-  <si>
-    <t>5369831207315ea5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.5db705c7ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:09+02:00</t>
+  </si>
+  <si>
+    <t>f139281423f67eac</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.78dae4b58b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT13_KO</t>
@@ -1228,13 +1228,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-02T17:57:46+02:00</t>
-  </si>
-  <si>
-    <t>16adfb877fb04483</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.0e2af359c3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:11+02:00</t>
+  </si>
+  <si>
+    <t>89ce3a3dfaea8046</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.3ca5994f43^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT14_KO</t>
@@ -1245,13 +1245,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-02T17:57:48+02:00</t>
-  </si>
-  <si>
-    <t>b95b3fb7ba667523</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.5727a3eda4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:13+02:00</t>
+  </si>
+  <si>
+    <t>2117f2a26e87b765</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.87108eae33^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT15_KO</t>
@@ -1262,13 +1262,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-02T17:57:50+02:00</t>
-  </si>
-  <si>
-    <t>bfece030bb7c6fe7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.d19f6f038f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:15+02:00</t>
+  </si>
+  <si>
+    <t>98d30326dfcf5d2b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.9664e50b2b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT16_KO</t>
@@ -1279,13 +1279,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-02T17:57:52+02:00</t>
-  </si>
-  <si>
-    <t>a0be71d9a15c35cf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.986dfd36d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:17+02:00</t>
+  </si>
+  <si>
+    <t>0d35d03d1c4f1f95</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.bfefd96dcd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT5_KO</t>
@@ -1296,13 +1296,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:53+02:00</t>
-  </si>
-  <si>
-    <t>208bbd41f54af9a5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.181e354485^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:19+02:00</t>
+  </si>
+  <si>
+    <t>2da172a78a3b2c90</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.5997ae39ce^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT6_KO</t>
@@ -1320,13 +1320,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:55+02:00</t>
-  </si>
-  <si>
-    <t>0a37dc49de2f8fb8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.289aac7f51^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:21+02:00</t>
+  </si>
+  <si>
+    <t>fadb9e362c5f1d1d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.5746eee286^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT8_KO</t>
@@ -1336,13 +1336,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:57+02:00</t>
-  </si>
-  <si>
-    <t>5335cfa03ff63292</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.42fe72bdbf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:23+02:00</t>
+  </si>
+  <si>
+    <t>e3d0f9112d695fab</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.fb5e98d64e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT9_KO</t>
@@ -1353,13 +1353,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:57:59+02:00</t>
-  </si>
-  <si>
-    <t>7bc83a069a48318f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.06bb4954b4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:25+02:00</t>
+  </si>
+  <si>
+    <t>1af715c2d6993977</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.0f2479635c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT10_KO</t>
@@ -1370,13 +1370,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:00+02:00</t>
-  </si>
-  <si>
-    <t>ca9399807fd104e4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.16eeec0621^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:27+02:00</t>
+  </si>
+  <si>
+    <t>b42e22771b12e336</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b7bd842f34^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT11_KO</t>
@@ -1387,13 +1387,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:02+02:00</t>
-  </si>
-  <si>
-    <t>fb84e2ea3c9a5ec4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.f55c7b8f6f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:29+02:00</t>
+  </si>
+  <si>
+    <t>9e77fc355bd16bf7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.25693a9ef5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT12_KO</t>
@@ -1404,13 +1404,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:04+02:00</t>
-  </si>
-  <si>
-    <t>b091e214eba9ad35</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.2aa8226b6e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:32+02:00</t>
+  </si>
+  <si>
+    <t>166f6fa9eac7a7d5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.e4e3a67c03^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT13_KO</t>
@@ -1420,13 +1420,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:06+02:00</t>
-  </si>
-  <si>
-    <t>75ab022118a943ac</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d8cd9aa509^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:34+02:00</t>
+  </si>
+  <si>
+    <t>2196c66c9881aa5b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d79495e320^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT14_KO</t>
@@ -1436,13 +1436,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:07+02:00</t>
-  </si>
-  <si>
-    <t>26777e55fe3e566b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d66109a612^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:37+02:00</t>
+  </si>
+  <si>
+    <t>f7e2891ac407e259</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.5628474148^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT15_KO</t>
@@ -1453,13 +1453,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:10+02:00</t>
-  </si>
-  <si>
-    <t>41842e9fc10c0760</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.c83de000cb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:39+02:00</t>
+  </si>
+  <si>
+    <t>5b8d2dd7a069f649</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.60234ad71f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT16_KO</t>
@@ -1470,13 +1470,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:12+02:00</t>
-  </si>
-  <si>
-    <t>863558cf098a0ec3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.23433fa939^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:41+02:00</t>
+  </si>
+  <si>
+    <t>54324cdc1ea7726f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.75a45bf108^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT17_KO</t>
@@ -1487,13 +1487,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:14+02:00</t>
-  </si>
-  <si>
-    <t>4df24a3ab6b56d07</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.4987e8dd27^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:43+02:00</t>
+  </si>
+  <si>
+    <t>e435b0ff6541a460</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.cca9be6e85^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT18_KO</t>
@@ -1504,13 +1504,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:16+02:00</t>
-  </si>
-  <si>
-    <t>8c2aee5458cb57e1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.5e26462cf7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:45+02:00</t>
+  </si>
+  <si>
+    <t>f8291661309c7397</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.7aba1b8b78^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT19_KO</t>
@@ -1520,13 +1520,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:17+02:00</t>
-  </si>
-  <si>
-    <t>a507200067e82524</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.15e9cee836^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:47+02:00</t>
+  </si>
+  <si>
+    <t>b72ffd74125357e8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b7a9fbfe97^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT20_KO</t>
@@ -1536,13 +1536,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:19+02:00</t>
-  </si>
-  <si>
-    <t>07747d9d4c5ef757</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.273999ee41^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:49+02:00</t>
+  </si>
+  <si>
+    <t>cc7c6b7ab245f8cc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.6a846544d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT21_KO</t>
@@ -1553,13 +1553,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:21+02:00</t>
-  </si>
-  <si>
-    <t>afaac2f5a4a7f8f4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.a61e583437^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:51+02:00</t>
+  </si>
+  <si>
+    <t>ef589664b611cfe8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.c2850840a0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT22_KO</t>
@@ -1570,13 +1570,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:23+02:00</t>
-  </si>
-  <si>
-    <t>ad76b4d03cfa4ecc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.1c6c129ca7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:54+02:00</t>
+  </si>
+  <si>
+    <t>5801d65d2ec14ec0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b7562039fa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT23_KO</t>
@@ -1587,13 +1587,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:24+02:00</t>
-  </si>
-  <si>
-    <t>241accf72ee6057c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b8b079bd0e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:56+02:00</t>
+  </si>
+  <si>
+    <t>d22f6cb94bcda556</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.de11232c6f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT5_KO</t>
@@ -2007,13 +2007,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-02T17:58:58+02:00</t>
-  </si>
-  <si>
-    <t>5b6071125ec0679a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.1ea252a196^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:35+02:00</t>
+  </si>
+  <si>
+    <t>08bdeab593f7f7f4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5e436ec088^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT2</t>
@@ -2025,13 +2025,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-02T17:59:00+02:00</t>
-  </si>
-  <si>
-    <t>af930d43e1e4968f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c60bbf120c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:37+02:00</t>
+  </si>
+  <si>
+    <t>dded70a3b6a6b7b3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.0ff6ebcf06^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT3</t>
@@ -2043,13 +2043,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-02T17:59:02+02:00</t>
-  </si>
-  <si>
-    <t>16cd1bdb945814e8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.2857070f35^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:39+02:00</t>
+  </si>
+  <si>
+    <t>1c8cb8bac2383721</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5116dbb166^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT4</t>
@@ -2061,13 +2061,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-02T17:59:04+02:00</t>
-  </si>
-  <si>
-    <t>66b46f9a7f1c30e0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.b8b1dc4788^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:42+02:00</t>
+  </si>
+  <si>
+    <t>657a194b5daef640</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.62b41f1b0a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT5_KO</t>
@@ -2077,13 +2077,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:26+02:00</t>
-  </si>
-  <si>
-    <t>42ed6e0e1e9443be</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.687857d670^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:52:58+02:00</t>
+  </si>
+  <si>
+    <t>2d39d2542e00a215</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.615fd8fa23^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT6_KO</t>
@@ -2102,13 +2102,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:28+02:00</t>
-  </si>
-  <si>
-    <t>a05aa83ce6c8bbbb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.d21787a681^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:00+02:00</t>
+  </si>
+  <si>
+    <t>0afd86ef4905aeb8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.d83946ff8d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT8_KO</t>
@@ -2119,13 +2119,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:29+02:00</t>
-  </si>
-  <si>
-    <t>84c3273212a404cc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.ed6a5b0589^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:02+02:00</t>
+  </si>
+  <si>
+    <t>302831371fcd1a67</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.e3d9fd1353^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT9_KO</t>
@@ -2136,13 +2136,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:32+02:00</t>
-  </si>
-  <si>
-    <t>514686b088af1c69</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.ed51f403a0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:04+02:00</t>
+  </si>
+  <si>
+    <t>1623a71a821e6776</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.4de72efec4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT10_KO</t>
@@ -2153,13 +2153,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:34+02:00</t>
-  </si>
-  <si>
-    <t>561df35a74756d43</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.518acbc4cb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:06+02:00</t>
+  </si>
+  <si>
+    <t>5745d8dedc9c4c16</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.e141a08c52^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT11_KO</t>
@@ -2170,13 +2170,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:35+02:00</t>
-  </si>
-  <si>
-    <t>14b964d574cbcc9e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.789775c3f1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:08+02:00</t>
+  </si>
+  <si>
+    <t>c30fefb6944e7903</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.e5dab63ccf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT12_KO</t>
@@ -2187,13 +2187,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:37+02:00</t>
-  </si>
-  <si>
-    <t>c90a5ec4ffe8e901</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5cb23ca923^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:10+02:00</t>
+  </si>
+  <si>
+    <t>d9c000e47ecf0a25</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.9bea4563b7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT13_KO</t>
@@ -2203,13 +2203,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:39+02:00</t>
-  </si>
-  <si>
-    <t>9d7a89c6f271a0c2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.227ddd8d66^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:12+02:00</t>
+  </si>
+  <si>
+    <t>af66737339a1c81f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.34fab38dfe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT14_KO</t>
@@ -2219,13 +2219,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:41+02:00</t>
-  </si>
-  <si>
-    <t>1c704d9b345357bc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.604734fa47^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:14+02:00</t>
+  </si>
+  <si>
+    <t>77f0ccce630ec499</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.e9c4b23fc2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT15_KO</t>
@@ -2236,13 +2236,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:42+02:00</t>
-  </si>
-  <si>
-    <t>129406cd8882f40c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.61df45a12b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:17+02:00</t>
+  </si>
+  <si>
+    <t>2cf6648e91bce6d2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5dfca9649c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT16_KO</t>
@@ -2253,13 +2253,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:44+02:00</t>
-  </si>
-  <si>
-    <t>02ebb1bb3d74c8f6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.599358719b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:19+02:00</t>
+  </si>
+  <si>
+    <t>5e8b61e8952eb881</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.22c0804ada^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT17_KO</t>
@@ -2270,13 +2270,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:46+02:00</t>
-  </si>
-  <si>
-    <t>0f81546819e32ba6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.7e5c5b5bce^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:21+02:00</t>
+  </si>
+  <si>
+    <t>34a7d892192e3d63</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.19856677fa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT18_KO</t>
@@ -2287,13 +2287,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:48+02:00</t>
-  </si>
-  <si>
-    <t>5a636ba6b0f204e3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.ec770971a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:23+02:00</t>
+  </si>
+  <si>
+    <t>7100822c8eeaf055</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.b925619e01^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT19_KO</t>
@@ -2304,13 +2304,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:49+02:00</t>
-  </si>
-  <si>
-    <t>8c46a5ade198aff4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.36b49ef7e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:25+02:00</t>
+  </si>
+  <si>
+    <t>1195797d29398d70</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.dc3a6af0ee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT20_KO</t>
@@ -2321,13 +2321,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:51+02:00</t>
-  </si>
-  <si>
-    <t>ed05bc26fee47d97</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.38000c4401^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:27+02:00</t>
+  </si>
+  <si>
+    <t>a418fb3bdf234402</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.3636b02a52^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT21_KO</t>
@@ -2338,13 +2338,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:53+02:00</t>
-  </si>
-  <si>
-    <t>daa28e032f7b6c95</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.b90d411753^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:29+02:00</t>
+  </si>
+  <si>
+    <t>abbcab9709019cd5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.86b9d182da^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT22_KO</t>
@@ -2355,13 +2355,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:55+02:00</t>
-  </si>
-  <si>
-    <t>9da30ca5d7fe3117</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.188679481b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:31+02:00</t>
+  </si>
+  <si>
+    <t>175e7b65975da8fa</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.6ca7783348^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT23_KO</t>
@@ -2372,13 +2372,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:58:56+02:00</t>
-  </si>
-  <si>
-    <t>d8f60ae069419e8b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.987e775898^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:33+02:00</t>
+  </si>
+  <si>
+    <t>424dcc419db32587</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.318acfa890^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_PSS_CT1</t>
@@ -2560,13 +2560,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-02T17:59:05+02:00</t>
-  </si>
-  <si>
-    <t>f39a50fc1890d758</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.d892ce756c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:44+02:00</t>
+  </si>
+  <si>
+    <t>83b6f8db5debcf7f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.07df0fc463^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>PUBBLICAZIONE_CREAZIONE</t>
@@ -4560,13 +4560,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-02T17:59:07+02:00</t>
-  </si>
-  <si>
-    <t>a76abb028527122a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a8f09a2206^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:46+02:00</t>
+  </si>
+  <si>
+    <t>76c0e63f8c3d080b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.5e520d3f10^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT0</t>
@@ -4577,13 +4577,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:59:09+02:00</t>
-  </si>
-  <si>
-    <t>8048fe8c2bc50ac9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.46e92dcc10^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:48+02:00</t>
+  </si>
+  <si>
+    <t>06ab878c6fe0c404</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.1b85360b6d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT0</t>
@@ -4594,13 +4594,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-02T17:59:11+02:00</t>
-  </si>
-  <si>
-    <t>3fb029f33990bff4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.f9961af97f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:50+02:00</t>
+  </si>
+  <si>
+    <t>7be3959a3751a30f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.f760f5a6db^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT0</t>
@@ -4636,13 +4636,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-02T17:59:13+02:00</t>
-  </si>
-  <si>
-    <t>04d1382bd530100d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.4b1f94c4cf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-09T17:53:52+02:00</t>
+  </si>
+  <si>
+    <t>621dca976044da1b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.3b194ed64b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_PSS_CT0</t>
@@ -4652,24 +4652,6 @@
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 Il Documento CDA2 Profilo Sanitario Sintetico dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test PSS" e "CDA2_Profilo_Sanitario_Sintetico_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
 </t>
-  </si>
-  <si>
-    <t>VALIDAZIONE_CDA2_LAB_TRASF_CT2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-Il Documento CDA2 Laboratorio dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST OK - HLA" riportata nei documenti "Caso di test - Trasfusionale" e "CDA2_Trasfusionale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
-</t>
-  </si>
-  <si>
-    <t>2023-08-02T17:59:14+02:00</t>
-  </si>
-  <si>
-    <t>32a58c44dfe13150</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.39e3e0a4e3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ID TEST CASE OK</t>
@@ -7758,7 +7740,7 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <pane xSplit="1" ySplit="40" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="376" topLeftCell="B377" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
@@ -9114,7 +9096,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:20" customHeight="1" ht="131">
+    <row r="36" spans="1:20" customHeight="1" ht="145.5">
       <c r="A36" s="20">
         <v>29</v>
       </c>
@@ -9228,7 +9210,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="1:20" customHeight="1" ht="131">
+    <row r="39" spans="1:20" customHeight="1" ht="145.5">
       <c r="A39" s="20">
         <v>32</v>
       </c>
@@ -23519,36 +23501,16 @@
       </c>
     </row>
     <row r="383" spans="1:20" customHeight="1" ht="14.25">
-      <c r="A383" s="20">
-        <v>376</v>
-      </c>
-      <c r="B383" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C383" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D383" s="21" t="s">
-        <v>1044</v>
-      </c>
-      <c r="E383" s="22" t="s">
-        <v>1045</v>
-      </c>
-      <c r="F383" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G383" s="24" t="s">
-        <v>1046</v>
-      </c>
-      <c r="H383" s="24" t="s">
-        <v>1047</v>
-      </c>
-      <c r="I383" s="24" t="s">
-        <v>1048</v>
-      </c>
-      <c r="J383" s="25" t="s">
-        <v>56</v>
-      </c>
+      <c r="A383" s="20"/>
+      <c r="B383" s="21"/>
+      <c r="C383" s="21"/>
+      <c r="D383" s="21"/>
+      <c r="E383" s="22"/>
+      <c r="F383" s="23"/>
+      <c r="G383" s="24"/>
+      <c r="H383" s="24"/>
+      <c r="I383" s="24"/>
+      <c r="J383" s="25"/>
       <c r="K383" s="25"/>
       <c r="L383" s="25"/>
       <c r="M383" s="25"/>
@@ -23557,12 +23519,8 @@
       <c r="P383" s="25"/>
       <c r="Q383" s="25"/>
       <c r="R383" s="26"/>
-      <c r="S383" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="T383" s="28" t="s">
-        <v>58</v>
-      </c>
+      <c r="S383" s="27"/>
+      <c r="T383" s="28"/>
     </row>
     <row r="384" spans="1:20" customHeight="1" ht="14.25">
       <c r="F384" s="12"/>
@@ -28271,10 +28229,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>1049</v>
+        <v>1044</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>1050</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="2" spans="1:6" customHeight="1" ht="14.25">
@@ -28282,13 +28240,13 @@
         <v>49</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>1051</v>
+        <v>1046</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>1052</v>
+        <v>1047</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>1053</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="3" spans="1:6" customHeight="1" ht="14.25">
@@ -28296,13 +28254,13 @@
         <v>79</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>1051</v>
+        <v>1046</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>1054</v>
+        <v>1049</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>1055</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="4" spans="1:6" customHeight="1" ht="14.25">
@@ -28310,13 +28268,13 @@
         <v>100</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>1051</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>1056</v>
-      </c>
       <c r="D4" s="31" t="s">
-        <v>1057</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="5" spans="1:6" customHeight="1" ht="14.25">
@@ -28324,13 +28282,13 @@
         <v>121</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>1051</v>
+        <v>1046</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>1058</v>
+        <v>1053</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>1059</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="6" spans="1:6" customHeight="1" ht="14.25">
@@ -28338,13 +28296,13 @@
         <v>132</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>1051</v>
+        <v>1046</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>1060</v>
+        <v>1055</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>1061</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="7" spans="1:6" customHeight="1" ht="14.5">
@@ -28352,13 +28310,13 @@
         <v>141</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>1051</v>
+        <v>1046</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>1062</v>
+        <v>1057</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>1063</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="8" spans="1:6" customHeight="1" ht="14.5">
@@ -28366,13 +28324,13 @@
         <v>159</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>1051</v>
+        <v>1046</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>1064</v>
+        <v>1059</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>1065</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="9" spans="1:6" customHeight="1" ht="14.5">
@@ -28380,27 +28338,27 @@
         <v>155</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>1051</v>
+        <v>1046</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>1066</v>
+        <v>1061</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>1067</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="10" spans="1:6" customHeight="1" ht="43.5">
       <c r="A10" s="11" t="s">
-        <v>1068</v>
+        <v>1063</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>1051</v>
+        <v>1046</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>1069</v>
+        <v>1064</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>1070</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="11" spans="1:6" customHeight="1" ht="14.25">
@@ -28408,13 +28366,13 @@
         <v>49</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>1071</v>
+        <v>1066</v>
       </c>
       <c r="C11" s="30">
         <v>192</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>1072</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="12" spans="1:6" customHeight="1" ht="14.25">
@@ -28422,13 +28380,13 @@
         <v>79</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>1071</v>
+        <v>1066</v>
       </c>
       <c r="C12" s="30">
         <v>208</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>1073</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="13" spans="1:6" customHeight="1" ht="14.25">
@@ -28436,13 +28394,13 @@
         <v>100</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>1071</v>
+        <v>1066</v>
       </c>
       <c r="C13" s="30">
         <v>224</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>1074</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="14" spans="1:6" customHeight="1" ht="14.25">
@@ -28450,13 +28408,13 @@
         <v>121</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>1071</v>
+        <v>1066</v>
       </c>
       <c r="C14" s="30">
         <v>240</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>1075</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="15" spans="1:6" customHeight="1" ht="14.25">
@@ -28464,13 +28422,13 @@
         <v>132</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>1071</v>
+        <v>1066</v>
       </c>
       <c r="C15" s="30">
         <v>256</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>1076</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="16" spans="1:6" customHeight="1" ht="14.25">
@@ -28478,13 +28436,13 @@
         <v>141</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>1071</v>
+        <v>1066</v>
       </c>
       <c r="C16" s="30">
         <v>272</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>1077</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="17" spans="1:6" customHeight="1" ht="14.25">
@@ -28492,13 +28450,13 @@
         <v>159</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>1071</v>
+        <v>1066</v>
       </c>
       <c r="C17" s="30">
         <v>288</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>1078</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="18" spans="1:6" customHeight="1" ht="13.5">
@@ -28506,13 +28464,13 @@
         <v>155</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>1071</v>
+        <v>1066</v>
       </c>
       <c r="C18" s="30">
         <v>304</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>1079</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="19" spans="1:6" customHeight="1" ht="14.25">
@@ -28520,13 +28478,13 @@
         <v>49</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
       <c r="C19" s="30">
         <v>193</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>1081</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="20" spans="1:6" customHeight="1" ht="14.25">
@@ -28534,13 +28492,13 @@
         <v>79</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
       <c r="C20" s="30">
         <v>209</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>1082</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="21" spans="1:6" customHeight="1" ht="14.25">
@@ -28548,13 +28506,13 @@
         <v>100</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
       <c r="C21" s="30">
         <v>225</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>1083</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="22" spans="1:6" customHeight="1" ht="14.25">
@@ -28562,13 +28520,13 @@
         <v>121</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
       <c r="C22" s="30">
         <v>241</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>1084</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="23" spans="1:6" customHeight="1" ht="14.25">
@@ -28576,13 +28534,13 @@
         <v>132</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
       <c r="C23" s="30">
         <v>257</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>1085</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="24" spans="1:6" customHeight="1" ht="14.25">
@@ -28590,13 +28548,13 @@
         <v>141</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
       <c r="C24" s="30">
         <v>273</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>1086</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="25" spans="1:6" customHeight="1" ht="14.25">
@@ -28604,13 +28562,13 @@
         <v>159</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
       <c r="C25" s="30">
         <v>289</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>1087</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="26" spans="1:6" customHeight="1" ht="14.25">
@@ -28618,13 +28576,13 @@
         <v>155</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
       <c r="C26" s="30">
         <v>305</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>1088</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="27" spans="1:6" customHeight="1" ht="14.25">
@@ -28632,13 +28590,13 @@
         <v>49</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>1089</v>
+        <v>1084</v>
       </c>
       <c r="C27" s="30">
         <v>194</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>1090</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="28" spans="1:6" customHeight="1" ht="14.25">
@@ -28646,13 +28604,13 @@
         <v>79</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>1089</v>
+        <v>1084</v>
       </c>
       <c r="C28" s="30">
         <v>210</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>1091</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="29" spans="1:6" customHeight="1" ht="14.25">
@@ -28660,13 +28618,13 @@
         <v>100</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>1089</v>
+        <v>1084</v>
       </c>
       <c r="C29" s="30">
         <v>226</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>1092</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="30" spans="1:6" customHeight="1" ht="14.25">
@@ -28674,13 +28632,13 @@
         <v>121</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>1089</v>
+        <v>1084</v>
       </c>
       <c r="C30" s="30">
         <v>242</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>1093</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="31" spans="1:6" customHeight="1" ht="14.25">
@@ -28688,13 +28646,13 @@
         <v>132</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>1089</v>
+        <v>1084</v>
       </c>
       <c r="C31" s="30">
         <v>258</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>1094</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="32" spans="1:6" customHeight="1" ht="14.25">
@@ -28702,13 +28660,13 @@
         <v>141</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>1089</v>
+        <v>1084</v>
       </c>
       <c r="C32" s="30">
         <v>274</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>1095</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="33" spans="1:6" customHeight="1" ht="14.25">
@@ -28716,13 +28674,13 @@
         <v>159</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>1089</v>
+        <v>1084</v>
       </c>
       <c r="C33" s="30">
         <v>290</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>1096</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="34" spans="1:6" customHeight="1" ht="14.25">
@@ -28730,13 +28688,13 @@
         <v>155</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>1089</v>
+        <v>1084</v>
       </c>
       <c r="C34" s="30">
         <v>306</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>1097</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="35" spans="1:6" customHeight="1" ht="14.25">
@@ -28744,7 +28702,7 @@
         <v>49</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>1098</v>
+        <v>1093</v>
       </c>
       <c r="C35" s="30">
         <v>195</v>
@@ -28758,7 +28716,7 @@
         <v>79</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>1098</v>
+        <v>1093</v>
       </c>
       <c r="C36" s="30">
         <v>211</v>
@@ -28772,7 +28730,7 @@
         <v>100</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>1098</v>
+        <v>1093</v>
       </c>
       <c r="C37" s="30">
         <v>227</v>
@@ -28786,7 +28744,7 @@
         <v>121</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>1098</v>
+        <v>1093</v>
       </c>
       <c r="C38" s="30">
         <v>243</v>
@@ -28800,7 +28758,7 @@
         <v>132</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>1098</v>
+        <v>1093</v>
       </c>
       <c r="C39" s="30">
         <v>259</v>
@@ -28814,7 +28772,7 @@
         <v>141</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>1098</v>
+        <v>1093</v>
       </c>
       <c r="C40" s="30">
         <v>275</v>
@@ -28828,7 +28786,7 @@
         <v>159</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>1098</v>
+        <v>1093</v>
       </c>
       <c r="C41" s="30">
         <v>291</v>
@@ -28842,7 +28800,7 @@
         <v>155</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>1098</v>
+        <v>1093</v>
       </c>
       <c r="C42" s="30">
         <v>307</v>
@@ -28856,7 +28814,7 @@
         <v>49</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>1099</v>
+        <v>1094</v>
       </c>
       <c r="C43" s="30">
         <v>196</v>
@@ -28870,7 +28828,7 @@
         <v>79</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>1099</v>
+        <v>1094</v>
       </c>
       <c r="C44" s="30">
         <v>212</v>
@@ -28884,7 +28842,7 @@
         <v>100</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>1099</v>
+        <v>1094</v>
       </c>
       <c r="C45" s="30">
         <v>228</v>
@@ -28898,7 +28856,7 @@
         <v>121</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>1099</v>
+        <v>1094</v>
       </c>
       <c r="C46" s="30">
         <v>244</v>
@@ -28912,7 +28870,7 @@
         <v>132</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>1099</v>
+        <v>1094</v>
       </c>
       <c r="C47" s="30">
         <v>260</v>
@@ -28926,7 +28884,7 @@
         <v>141</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>1099</v>
+        <v>1094</v>
       </c>
       <c r="C48" s="30">
         <v>276</v>
@@ -28940,7 +28898,7 @@
         <v>159</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>1099</v>
+        <v>1094</v>
       </c>
       <c r="C49" s="30">
         <v>292</v>
@@ -28954,7 +28912,7 @@
         <v>155</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>1099</v>
+        <v>1094</v>
       </c>
       <c r="C50" s="30">
         <v>308</v>
@@ -29960,7 +29918,7 @@
     </row>
     <row r="2" spans="1:6" customHeight="1" ht="14.25">
       <c r="A2" s="4" t="s">
-        <v>1100</v>
+        <v>1095</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>56</v>
@@ -29968,7 +29926,7 @@
     </row>
     <row r="3" spans="1:6" customHeight="1" ht="14.25">
       <c r="A3" s="4" t="s">
-        <v>1101</v>
+        <v>1096</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>124</v>

</xml_diff>

<commit_message>
fix: adeguamenti mancato accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SPEITSRL/SPE.IT s.r.l/FSE INI Adapter/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111SPEITSRL/SPE.IT s.r.l/FSE INI Adapter/1.0/report-checklist.xlsx
@@ -333,16 +333,16 @@
 </t>
   </si>
   <si>
-    <t>09/08/2023</t>
-  </si>
-  <si>
-    <t>2023-08-09T17:50:58+02:00</t>
-  </si>
-  <si>
-    <t>ff990bea1a322f0c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.e34a1fab6a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>22/08/2023</t>
+  </si>
+  <si>
+    <t>2023-08-22T08:54:46+02:00</t>
+  </si>
+  <si>
+    <t>45e7d0d2d37feeba</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.e2dcdb39d1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -363,13 +363,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-09T17:51:01+02:00</t>
-  </si>
-  <si>
-    <t>233492747b5e55c0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.3eb3ee7101^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:54:49+02:00</t>
+  </si>
+  <si>
+    <t>f7a2a3179e7629df</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.df1bb8c722^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT3</t>
@@ -381,13 +381,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-09T17:51:03+02:00</t>
-  </si>
-  <si>
-    <t>b658e07d4ec49f3c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.adeb01a5aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:54:52+02:00</t>
+  </si>
+  <si>
+    <t>4ea7b7e66bb10661</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.d35c67138a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT4</t>
@@ -399,13 +399,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-09T17:51:05+02:00</t>
-  </si>
-  <si>
-    <t>95583b99165f575f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.4d43c16813^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:54:55+02:00</t>
+  </si>
+  <si>
+    <t>d8345ffe2db1d7ea</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.2a03f83235^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT5</t>
@@ -417,13 +417,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-09T17:51:07+02:00</t>
-  </si>
-  <si>
-    <t>229dc8493b43b728</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.7f5d619b19^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:54:58+02:00</t>
+  </si>
+  <si>
+    <t>2c92aa654b0c743a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.6e20948fc5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>LDO</t>
@@ -437,13 +437,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:09+02:00</t>
-  </si>
-  <si>
-    <t>66bb6eec1c6d641f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.98f7e0cec0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:01+02:00</t>
+  </si>
+  <si>
+    <t>2b97138b5b8bc081</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.63bb462e0e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT2</t>
@@ -454,13 +454,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:11+02:00</t>
-  </si>
-  <si>
-    <t>1297c717f82d1d22</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.5f5012873d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:04+02:00</t>
+  </si>
+  <si>
+    <t>bb2e12bfac1770ee</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.09900257ff^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT3</t>
@@ -471,13 +471,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:13+02:00</t>
-  </si>
-  <si>
-    <t>e15879cac42b117b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.3ea6da98df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:07+02:00</t>
+  </si>
+  <si>
+    <t>5e20330b19ce26df</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.57a345c8ee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT4</t>
@@ -488,13 +488,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:15+02:00</t>
-  </si>
-  <si>
-    <t>448fe0844a6ef5f2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.b971e897de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:10+02:00</t>
+  </si>
+  <si>
+    <t>4492e6997d8450bf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.5ec0a0193c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>RAD</t>
@@ -508,13 +508,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:18+02:00</t>
-  </si>
-  <si>
-    <t>184a60cc80e70db1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.8c13dc732a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:13+02:00</t>
+  </si>
+  <si>
+    <t>e833067ec310d927</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.4179d39142^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT2</t>
@@ -525,13 +525,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:20+02:00</t>
-  </si>
-  <si>
-    <t>43d0be61ed35e02a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.a09163b23b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:16+02:00</t>
+  </si>
+  <si>
+    <t>cf56c04a640a8af6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.dd94cff83f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT3</t>
@@ -542,13 +542,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:22+02:00</t>
-  </si>
-  <si>
-    <t>fcf858dcf077f452</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.bf6230c4df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:19+02:00</t>
+  </si>
+  <si>
+    <t>5367d6f7b9a6ddbf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.4e93eec30b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT4</t>
@@ -559,13 +559,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:24+02:00</t>
-  </si>
-  <si>
-    <t>5dab3157b255f84a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.8dc02c8ceb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:22+02:00</t>
+  </si>
+  <si>
+    <t>675e122ee133278c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.1755980587^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>CERT_VAC</t>
@@ -829,10 +829,10 @@
     </r>
   </si>
   <si>
-    <t>2023-08-09T17:51:26+02:00</t>
-  </si>
-  <si>
-    <t>3f99a0b7f2a193e6</t>
+    <t>2023-08-22T08:55:25+02:00</t>
+  </si>
+  <si>
+    <t>1ad07bd7ba73595b</t>
   </si>
   <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
@@ -847,10 +847,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:29+02:00</t>
-  </si>
-  <si>
-    <t>08761ab3bf9e3ad2</t>
+    <t>2023-08-22T08:55:28+02:00</t>
+  </si>
+  <si>
+    <t>c485d66b5c88433c</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_PSS_KO</t>
@@ -859,19 +859,19 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RAD_KO</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:31+02:00</t>
-  </si>
-  <si>
-    <t>db0b03df7758bd2a</t>
+    <t>2023-08-22T08:55:31+02:00</t>
+  </si>
+  <si>
+    <t>32781d09b4f57897</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:33+02:00</t>
-  </si>
-  <si>
-    <t>f926021cfda0e2eb</t>
+    <t>2023-08-22T08:55:34+02:00</t>
+  </si>
+  <si>
+    <t>11731e3c5cd22939</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_CERT_VAC_KO</t>
@@ -921,13 +921,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:35+02:00</t>
-  </si>
-  <si>
-    <t>013fa11e746877ec</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.1222b8109c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:36+02:00</t>
+  </si>
+  <si>
+    <t>8377c188cc3ac004</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a3aadeda9e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore di sintassi.</t>
@@ -950,13 +950,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:37+02:00</t>
-  </si>
-  <si>
-    <t>4c2f604cafcd775f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a21a1909a2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:39+02:00</t>
+  </si>
+  <si>
+    <t>d92e4a8aac89f24c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.ffa23a481b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore semantico.</t>
@@ -969,13 +969,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:39+02:00</t>
-  </si>
-  <si>
-    <t>110c2c0cadafadb7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.7da2cae15d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:42+02:00</t>
+  </si>
+  <si>
+    <t>7d9ccdaefa19fcdf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.61250ddf1a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT10_KO</t>
@@ -985,13 +985,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:41+02:00</t>
-  </si>
-  <si>
-    <t>9f4edf35f336735b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.f3b8431904^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:45+02:00</t>
+  </si>
+  <si>
+    <t>140fdddf1a0b91cd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.96b1e11918^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT11_KO</t>
@@ -1001,13 +1001,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:43+02:00</t>
-  </si>
-  <si>
-    <t>a70062f16f7023c4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.6c46179b61^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:48+02:00</t>
+  </si>
+  <si>
+    <t>096bf31c4bfd529a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.e9f5178d6f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore vocabolario.</t>
@@ -1020,13 +1020,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:46+02:00</t>
-  </si>
-  <si>
-    <t>d3c639b368cc52db</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.8e661a1f50^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:51+02:00</t>
+  </si>
+  <si>
+    <t>185e078d1da272c6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.3f0b0a4da3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT13_KO</t>
@@ -1036,13 +1036,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:48+02:00</t>
-  </si>
-  <si>
-    <t>08cae0e036da3356</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.d7ed938e18^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:54+02:00</t>
+  </si>
+  <si>
+    <t>abc817132da31530</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.bd5d29ee08^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT14_KO</t>
@@ -1052,13 +1052,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:50+02:00</t>
-  </si>
-  <si>
-    <t>6dcddfe4a1e001bc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.00e8e03982^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:55:57+02:00</t>
+  </si>
+  <si>
+    <t>8a3bee0f3b623b69</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a1a4415591^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT15_KO</t>
@@ -1068,13 +1068,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:52+02:00</t>
-  </si>
-  <si>
-    <t>f41fcc47453a7192</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.6f94ec95c5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:00+02:00</t>
+  </si>
+  <si>
+    <t>ac9786fa7456289d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.5eab687991^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT16_KO</t>
@@ -1084,13 +1084,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:51:54+02:00</t>
-  </si>
-  <si>
-    <t>662266052a49f579</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.b92cd78908^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:03+02:00</t>
+  </si>
+  <si>
+    <t>bc9634491700430c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.f094a7a94d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT5_KO</t>
@@ -1101,13 +1101,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-09T17:51:56+02:00</t>
-  </si>
-  <si>
-    <t>270048e2de5cccfd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.770c0a0afd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:06+02:00</t>
+  </si>
+  <si>
+    <t>26c969746b5d4b2a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.752148eb17^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT6_KO</t>
@@ -1126,13 +1126,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-09T17:51:58+02:00</t>
-  </si>
-  <si>
-    <t>f279c095246a41ca</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.75e69533f6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:09+02:00</t>
+  </si>
+  <si>
+    <t>09d680fff5421349</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.734d641789^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT8_KO</t>
@@ -1143,13 +1143,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-09T17:52:00+02:00</t>
-  </si>
-  <si>
-    <t>4172635a2cba6aab</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.b2cf82d636^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:12+02:00</t>
+  </si>
+  <si>
+    <t>0db1f9441993332e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.158a6a5850^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT9_KO</t>
@@ -1160,13 +1160,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-09T17:52:02+02:00</t>
-  </si>
-  <si>
-    <t>6b8896078ef38bb8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.770a11571b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:15+02:00</t>
+  </si>
+  <si>
+    <t>5407f62d417de31a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.e4a6239e5b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT10_KO</t>
@@ -1177,13 +1177,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-09T17:52:04+02:00</t>
-  </si>
-  <si>
-    <t>d5e5b5cd3fbf6900</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.fd13a223a4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:18+02:00</t>
+  </si>
+  <si>
+    <t>59dbd493c9e0a7ef</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.860e734981^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT11_KO</t>
@@ -1194,13 +1194,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-09T17:52:06+02:00</t>
-  </si>
-  <si>
-    <t>e4174148d987259e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.5c196344e0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:21+02:00</t>
+  </si>
+  <si>
+    <t>bea8bf3d43422d49</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.5c33390d7f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT12_KO</t>
@@ -1211,13 +1211,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-09T17:52:09+02:00</t>
-  </si>
-  <si>
-    <t>f139281423f67eac</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.78dae4b58b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:24+02:00</t>
+  </si>
+  <si>
+    <t>cfbfb2d894fe559e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.8e18217075^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT13_KO</t>
@@ -1228,13 +1228,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-09T17:52:11+02:00</t>
-  </si>
-  <si>
-    <t>89ce3a3dfaea8046</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.3ca5994f43^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:27+02:00</t>
+  </si>
+  <si>
+    <t>dd7c1626a0dda725</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.7864fa584c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT14_KO</t>
@@ -1245,13 +1245,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-09T17:52:13+02:00</t>
-  </si>
-  <si>
-    <t>2117f2a26e87b765</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.87108eae33^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:30+02:00</t>
+  </si>
+  <si>
+    <t>4cac115d5fe5f91c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.ba0a2529c6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT15_KO</t>
@@ -1262,13 +1262,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-09T17:52:15+02:00</t>
-  </si>
-  <si>
-    <t>98d30326dfcf5d2b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.9664e50b2b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:33+02:00</t>
+  </si>
+  <si>
+    <t>bc204637e6b47dbc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.f01be87372^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT16_KO</t>
@@ -1279,13 +1279,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-09T17:52:17+02:00</t>
-  </si>
-  <si>
-    <t>0d35d03d1c4f1f95</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.bfefd96dcd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:36+02:00</t>
+  </si>
+  <si>
+    <t>6c02f515f1dc5250</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.e26ea0370b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT5_KO</t>
@@ -1296,13 +1296,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:19+02:00</t>
-  </si>
-  <si>
-    <t>2da172a78a3b2c90</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.5997ae39ce^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:39+02:00</t>
+  </si>
+  <si>
+    <t>f61de6cf7e294dd3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.3f5263378e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT6_KO</t>
@@ -1320,13 +1320,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:21+02:00</t>
-  </si>
-  <si>
-    <t>fadb9e362c5f1d1d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.5746eee286^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:41+02:00</t>
+  </si>
+  <si>
+    <t>e2242e1c44a81048</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.fe1c3552bd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT8_KO</t>
@@ -1336,13 +1336,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:23+02:00</t>
-  </si>
-  <si>
-    <t>e3d0f9112d695fab</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.fb5e98d64e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:45+02:00</t>
+  </si>
+  <si>
+    <t>90f75243211e6d1c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d021e1ea3e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT9_KO</t>
@@ -1353,13 +1353,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:25+02:00</t>
-  </si>
-  <si>
-    <t>1af715c2d6993977</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.0f2479635c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:48+02:00</t>
+  </si>
+  <si>
+    <t>1d1464afc54cf501</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.7db2ab2074^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT10_KO</t>
@@ -1370,13 +1370,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:27+02:00</t>
-  </si>
-  <si>
-    <t>b42e22771b12e336</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b7bd842f34^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:51+02:00</t>
+  </si>
+  <si>
+    <t>4fdc019fcd138828</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b17c94cd65^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT11_KO</t>
@@ -1387,13 +1387,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:29+02:00</t>
-  </si>
-  <si>
-    <t>9e77fc355bd16bf7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.25693a9ef5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:54+02:00</t>
+  </si>
+  <si>
+    <t>524e2445f2eb7252</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.c95bc7d7e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT12_KO</t>
@@ -1404,13 +1404,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:32+02:00</t>
-  </si>
-  <si>
-    <t>166f6fa9eac7a7d5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.e4e3a67c03^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:56:57+02:00</t>
+  </si>
+  <si>
+    <t>192370ec22952ab9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.86251ac75e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT13_KO</t>
@@ -1420,13 +1420,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:34+02:00</t>
-  </si>
-  <si>
-    <t>2196c66c9881aa5b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d79495e320^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:00+02:00</t>
+  </si>
+  <si>
+    <t>9a2f16c3c7bc87ad</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.97ca206309^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT14_KO</t>
@@ -1436,13 +1436,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:37+02:00</t>
-  </si>
-  <si>
-    <t>f7e2891ac407e259</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.5628474148^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:03+02:00</t>
+  </si>
+  <si>
+    <t>e99e84486731f1ae</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b4f244a801^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT15_KO</t>
@@ -1453,13 +1453,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:39+02:00</t>
-  </si>
-  <si>
-    <t>5b8d2dd7a069f649</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.60234ad71f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:06+02:00</t>
+  </si>
+  <si>
+    <t>3d5df5feb25a9eca</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.70204ed3d9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT16_KO</t>
@@ -1470,13 +1470,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:41+02:00</t>
-  </si>
-  <si>
-    <t>54324cdc1ea7726f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.75a45bf108^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:09+02:00</t>
+  </si>
+  <si>
+    <t>eafd47e8bbc15911</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.a4a94b0a63^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT17_KO</t>
@@ -1487,13 +1487,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:43+02:00</t>
-  </si>
-  <si>
-    <t>e435b0ff6541a460</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.cca9be6e85^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:12+02:00</t>
+  </si>
+  <si>
+    <t>76c34d46fe2bc2b1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.5ba2e4d808^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT18_KO</t>
@@ -1504,13 +1504,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:45+02:00</t>
-  </si>
-  <si>
-    <t>f8291661309c7397</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.7aba1b8b78^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:15+02:00</t>
+  </si>
+  <si>
+    <t>fc2d006fd826747c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d1b2ff41ad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT19_KO</t>
@@ -1520,13 +1520,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:47+02:00</t>
-  </si>
-  <si>
-    <t>b72ffd74125357e8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b7a9fbfe97^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:18+02:00</t>
+  </si>
+  <si>
+    <t>f075012576ec8e5c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.64c642b4b6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT20_KO</t>
@@ -1536,13 +1536,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:49+02:00</t>
-  </si>
-  <si>
-    <t>cc7c6b7ab245f8cc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.6a846544d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:22+02:00</t>
+  </si>
+  <si>
+    <t>e43d30883ed1e1e3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.0ddcc4a2ff^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT21_KO</t>
@@ -1553,13 +1553,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:51+02:00</t>
-  </si>
-  <si>
-    <t>ef589664b611cfe8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.c2850840a0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:25+02:00</t>
+  </si>
+  <si>
+    <t>0e27e3dec7337175</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.8be1accccb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT22_KO</t>
@@ -1570,13 +1570,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:54+02:00</t>
-  </si>
-  <si>
-    <t>5801d65d2ec14ec0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b7562039fa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:28+02:00</t>
+  </si>
+  <si>
+    <t>08b78847030146d0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.0418c1cb11^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT23_KO</t>
@@ -1587,13 +1587,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:56+02:00</t>
-  </si>
-  <si>
-    <t>d22f6cb94bcda556</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.de11232c6f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:31+02:00</t>
+  </si>
+  <si>
+    <t>51a11fd8b03f5394</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.72ca2e24bc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT5_KO</t>
@@ -2007,13 +2007,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-09T17:53:35+02:00</t>
-  </si>
-  <si>
-    <t>08bdeab593f7f7f4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5e436ec088^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:29+02:00</t>
+  </si>
+  <si>
+    <t>3bc0ce383136953f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5daaaf4fbf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT2</t>
@@ -2025,13 +2025,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-09T17:53:37+02:00</t>
-  </si>
-  <si>
-    <t>dded70a3b6a6b7b3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.0ff6ebcf06^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:33+02:00</t>
+  </si>
+  <si>
+    <t>c8f31890112d5054</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.b07ab7b7da^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT3</t>
@@ -2043,13 +2043,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-09T17:53:39+02:00</t>
-  </si>
-  <si>
-    <t>1c8cb8bac2383721</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5116dbb166^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:36+02:00</t>
+  </si>
+  <si>
+    <t>5c825099182ed331</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.3bdb8a18c8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT4</t>
@@ -2061,13 +2061,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-09T17:53:42+02:00</t>
-  </si>
-  <si>
-    <t>657a194b5daef640</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.62b41f1b0a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:39+02:00</t>
+  </si>
+  <si>
+    <t>e88968e93166958e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.0abf125a24^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT5_KO</t>
@@ -2077,13 +2077,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:52:58+02:00</t>
-  </si>
-  <si>
-    <t>2d39d2542e00a215</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.615fd8fa23^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:34+02:00</t>
+  </si>
+  <si>
+    <t>84b96ff5c469b1f1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.0870375500^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT6_KO</t>
@@ -2102,13 +2102,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:00+02:00</t>
-  </si>
-  <si>
-    <t>0afd86ef4905aeb8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.d83946ff8d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:37+02:00</t>
+  </si>
+  <si>
+    <t>b9bbcf5abe9605d3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.6493759e2d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT8_KO</t>
@@ -2119,13 +2119,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:02+02:00</t>
-  </si>
-  <si>
-    <t>302831371fcd1a67</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.e3d9fd1353^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:40+02:00</t>
+  </si>
+  <si>
+    <t>05364ced6df7e5c5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.af4e89df39^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT9_KO</t>
@@ -2136,13 +2136,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:04+02:00</t>
-  </si>
-  <si>
-    <t>1623a71a821e6776</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.4de72efec4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:43+02:00</t>
+  </si>
+  <si>
+    <t>acd7448c639a2fdd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.08e3280f8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT10_KO</t>
@@ -2153,13 +2153,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:06+02:00</t>
-  </si>
-  <si>
-    <t>5745d8dedc9c4c16</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.e141a08c52^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:47+02:00</t>
+  </si>
+  <si>
+    <t>1e549c4dc1a58af8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.ad7bfb099c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT11_KO</t>
@@ -2170,13 +2170,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:08+02:00</t>
-  </si>
-  <si>
-    <t>c30fefb6944e7903</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.e5dab63ccf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:50+02:00</t>
+  </si>
+  <si>
+    <t>fa4317f69f47f30b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.f52ffcd376^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT12_KO</t>
@@ -2187,13 +2187,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:10+02:00</t>
-  </si>
-  <si>
-    <t>d9c000e47ecf0a25</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.9bea4563b7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:52+02:00</t>
+  </si>
+  <si>
+    <t>5452d47079dba473</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.a1a86dd04e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT13_KO</t>
@@ -2203,13 +2203,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:12+02:00</t>
-  </si>
-  <si>
-    <t>af66737339a1c81f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.34fab38dfe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:55+02:00</t>
+  </si>
+  <si>
+    <t>793825fa178a130c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.86605d107b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT14_KO</t>
@@ -2219,13 +2219,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:14+02:00</t>
-  </si>
-  <si>
-    <t>77f0ccce630ec499</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.e9c4b23fc2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:57:59+02:00</t>
+  </si>
+  <si>
+    <t>5cb4988c572bcd61</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c1a75b97a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT15_KO</t>
@@ -2236,13 +2236,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:17+02:00</t>
-  </si>
-  <si>
-    <t>2cf6648e91bce6d2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5dfca9649c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:02+02:00</t>
+  </si>
+  <si>
+    <t>b7b2c243378503f1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.33224f5d0d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT16_KO</t>
@@ -2253,13 +2253,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:19+02:00</t>
-  </si>
-  <si>
-    <t>5e8b61e8952eb881</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.22c0804ada^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:05+02:00</t>
+  </si>
+  <si>
+    <t>74e84c0bd544d956</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5614842fef^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT17_KO</t>
@@ -2270,13 +2270,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:21+02:00</t>
-  </si>
-  <si>
-    <t>34a7d892192e3d63</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.19856677fa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:08+02:00</t>
+  </si>
+  <si>
+    <t>ec4d503b52880f97</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c0fb5cbcd9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT18_KO</t>
@@ -2287,13 +2287,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:23+02:00</t>
-  </si>
-  <si>
-    <t>7100822c8eeaf055</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.b925619e01^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:11+02:00</t>
+  </si>
+  <si>
+    <t>1d89126b3fa41bfd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c0895d9d89^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT19_KO</t>
@@ -2304,13 +2304,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:25+02:00</t>
-  </si>
-  <si>
-    <t>1195797d29398d70</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.dc3a6af0ee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:14+02:00</t>
+  </si>
+  <si>
+    <t>264469fc074ff0ad</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.1d78515aef^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT20_KO</t>
@@ -2321,13 +2321,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:27+02:00</t>
-  </si>
-  <si>
-    <t>a418fb3bdf234402</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.3636b02a52^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:17+02:00</t>
+  </si>
+  <si>
+    <t>7ee1a26fe6211fea</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c9f5b43437^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT21_KO</t>
@@ -2338,13 +2338,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:29+02:00</t>
-  </si>
-  <si>
-    <t>abbcab9709019cd5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.86b9d182da^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:20+02:00</t>
+  </si>
+  <si>
+    <t>23011ce9977d72d6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c6034ccdf2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT22_KO</t>
@@ -2355,13 +2355,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:31+02:00</t>
-  </si>
-  <si>
-    <t>175e7b65975da8fa</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.6ca7783348^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:23+02:00</t>
+  </si>
+  <si>
+    <t>9739e999c6961ec9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.8ba9c678a7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT23_KO</t>
@@ -2372,13 +2372,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:33+02:00</t>
-  </si>
-  <si>
-    <t>424dcc419db32587</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.318acfa890^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:26+02:00</t>
+  </si>
+  <si>
+    <t>708258d8a4858280</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.fe03afd587^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_PSS_CT1</t>
@@ -2560,13 +2560,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-09T17:53:44+02:00</t>
-  </si>
-  <si>
-    <t>83b6f8db5debcf7f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.07df0fc463^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:42+02:00</t>
+  </si>
+  <si>
+    <t>6147a06e3f364529</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.6587b68f3c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>PUBBLICAZIONE_CREAZIONE</t>
@@ -4560,13 +4560,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-09T17:53:46+02:00</t>
-  </si>
-  <si>
-    <t>76c0e63f8c3d080b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.5e520d3f10^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:45+02:00</t>
+  </si>
+  <si>
+    <t>c4c10452c03549cc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.deeee125e2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT0</t>
@@ -4577,13 +4577,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:48+02:00</t>
-  </si>
-  <si>
-    <t>06ab878c6fe0c404</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.1b85360b6d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:48+02:00</t>
+  </si>
+  <si>
+    <t>c4fc2afafb333599</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.27261d7251^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT0</t>
@@ -4594,13 +4594,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-09T17:53:50+02:00</t>
-  </si>
-  <si>
-    <t>7be3959a3751a30f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.f760f5a6db^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:53+02:00</t>
+  </si>
+  <si>
+    <t>ed4211fb4b8dcf6e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.7837133fd2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT0</t>
@@ -4636,13 +4636,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-09T17:53:52+02:00</t>
-  </si>
-  <si>
-    <t>621dca976044da1b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.3b194ed64b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-22T08:58:56+02:00</t>
+  </si>
+  <si>
+    <t>df67496cc406f381</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.14d60e88aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_PSS_CT0</t>

</xml_diff>

<commit_message>
fix: correzioni mancato accreditamento (cambiata tipologia iniezione)
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SPEITSRL/SPE.IT s.r.l/FSE INI Adapter/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111SPEITSRL/SPE.IT s.r.l/FSE INI Adapter/1.0/report-checklist.xlsx
@@ -333,16 +333,16 @@
 </t>
   </si>
   <si>
-    <t>22/08/2023</t>
-  </si>
-  <si>
-    <t>2023-08-22T08:54:46+02:00</t>
-  </si>
-  <si>
-    <t>45e7d0d2d37feeba</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.e2dcdb39d1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>23/08/2023</t>
+  </si>
+  <si>
+    <t>2023-08-23T16:07:42+02:00</t>
+  </si>
+  <si>
+    <t>341bf8852c47e0a0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.c9a65a1289^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -363,13 +363,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-22T08:54:49+02:00</t>
-  </si>
-  <si>
-    <t>f7a2a3179e7629df</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.df1bb8c722^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:07:44+02:00</t>
+  </si>
+  <si>
+    <t>30547dded4536b2f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.c5cf49f0fe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT3</t>
@@ -381,13 +381,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-22T08:54:52+02:00</t>
-  </si>
-  <si>
-    <t>4ea7b7e66bb10661</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.d35c67138a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:07:45+02:00</t>
+  </si>
+  <si>
+    <t>04030118f81bc70c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.6d8c78dca4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT4</t>
@@ -399,13 +399,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-22T08:54:55+02:00</t>
-  </si>
-  <si>
-    <t>d8345ffe2db1d7ea</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.2a03f83235^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:07:47+02:00</t>
+  </si>
+  <si>
+    <t>fb99f4ca0c7a26ab</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.c944023e9e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT5</t>
@@ -417,13 +417,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-22T08:54:58+02:00</t>
-  </si>
-  <si>
-    <t>2c92aa654b0c743a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.6e20948fc5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:07:48+02:00</t>
+  </si>
+  <si>
+    <t>b9d13f58bfafae94</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a3e8ecd7a5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>LDO</t>
@@ -437,13 +437,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:01+02:00</t>
-  </si>
-  <si>
-    <t>2b97138b5b8bc081</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.63bb462e0e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:07:49+02:00</t>
+  </si>
+  <si>
+    <t>e438cc3d63ded9ec</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.a30fe8cc9c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT2</t>
@@ -454,13 +454,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:04+02:00</t>
-  </si>
-  <si>
-    <t>bb2e12bfac1770ee</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.09900257ff^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:07:51+02:00</t>
+  </si>
+  <si>
+    <t>ce693949e4072dad</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.96f21db2b1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT3</t>
@@ -471,13 +471,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:07+02:00</t>
-  </si>
-  <si>
-    <t>5e20330b19ce26df</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.57a345c8ee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:07:52+02:00</t>
+  </si>
+  <si>
+    <t>2b358ebe47ae2984</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.836b0a2a85^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT4</t>
@@ -488,13 +488,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:10+02:00</t>
-  </si>
-  <si>
-    <t>4492e6997d8450bf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.5ec0a0193c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:07:53+02:00</t>
+  </si>
+  <si>
+    <t>22a2be18301f2647</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.13c13aa5dc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>RAD</t>
@@ -508,13 +508,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:13+02:00</t>
-  </si>
-  <si>
-    <t>e833067ec310d927</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.4179d39142^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:07:55+02:00</t>
+  </si>
+  <si>
+    <t>70867a71a40accb9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.478ef55116^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT2</t>
@@ -525,13 +525,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:16+02:00</t>
-  </si>
-  <si>
-    <t>cf56c04a640a8af6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.dd94cff83f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:07:56+02:00</t>
+  </si>
+  <si>
+    <t>eb6f6e91f26c83ba</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.f159c6021f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT3</t>
@@ -542,13 +542,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:19+02:00</t>
-  </si>
-  <si>
-    <t>5367d6f7b9a6ddbf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.4e93eec30b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:07:57+02:00</t>
+  </si>
+  <si>
+    <t>2666fdb37f1229f4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.a44747687b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT4</t>
@@ -559,13 +559,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:22+02:00</t>
-  </si>
-  <si>
-    <t>675e122ee133278c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.1755980587^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:07:58+02:00</t>
+  </si>
+  <si>
+    <t>f9777d3b84865900</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.faa8a260b2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>CERT_VAC</t>
@@ -829,10 +829,10 @@
     </r>
   </si>
   <si>
-    <t>2023-08-22T08:55:25+02:00</t>
-  </si>
-  <si>
-    <t>1ad07bd7ba73595b</t>
+    <t>2023-08-23T16:08:00+02:00</t>
+  </si>
+  <si>
+    <t>76b551586e73da67</t>
   </si>
   <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
@@ -847,10 +847,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:28+02:00</t>
-  </si>
-  <si>
-    <t>c485d66b5c88433c</t>
+    <t>2023-08-23T16:08:01+02:00</t>
+  </si>
+  <si>
+    <t>843e65d8aceaf983</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_PSS_KO</t>
@@ -859,19 +859,19 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RAD_KO</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:31+02:00</t>
-  </si>
-  <si>
-    <t>32781d09b4f57897</t>
+    <t>2023-08-23T16:08:02+02:00</t>
+  </si>
+  <si>
+    <t>d68079ab8124526e</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:34+02:00</t>
-  </si>
-  <si>
-    <t>11731e3c5cd22939</t>
+    <t>2023-08-23T16:08:04+02:00</t>
+  </si>
+  <si>
+    <t>3b8650bb1dcff098</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_CERT_VAC_KO</t>
@@ -921,13 +921,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:36+02:00</t>
-  </si>
-  <si>
-    <t>8377c188cc3ac004</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a3aadeda9e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:05+02:00</t>
+  </si>
+  <si>
+    <t>e03d9f282b6acbf5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.abd81ad865^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore di sintassi.</t>
@@ -950,13 +950,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:39+02:00</t>
-  </si>
-  <si>
-    <t>d92e4a8aac89f24c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.ffa23a481b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:06+02:00</t>
+  </si>
+  <si>
+    <t>eb19221f7755dab6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.365925b685^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore semantico.</t>
@@ -969,13 +969,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:42+02:00</t>
-  </si>
-  <si>
-    <t>7d9ccdaefa19fcdf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.61250ddf1a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:07+02:00</t>
+  </si>
+  <si>
+    <t>815e638c4b16d43e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.1aa4b13381^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT10_KO</t>
@@ -985,13 +985,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:45+02:00</t>
-  </si>
-  <si>
-    <t>140fdddf1a0b91cd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.96b1e11918^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:08+02:00</t>
+  </si>
+  <si>
+    <t>9c3992b313ff7d7e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.f311a097b6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT11_KO</t>
@@ -1001,13 +1001,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:48+02:00</t>
-  </si>
-  <si>
-    <t>096bf31c4bfd529a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.e9f5178d6f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:10+02:00</t>
+  </si>
+  <si>
+    <t>f8b3523ec0958e25</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.502e7be704^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>Errore vocabolario.</t>
@@ -1020,13 +1020,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:51+02:00</t>
-  </si>
-  <si>
-    <t>185e078d1da272c6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.3f0b0a4da3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:11+02:00</t>
+  </si>
+  <si>
+    <t>606438aa7e7ac830</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.922f291cce^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT13_KO</t>
@@ -1036,13 +1036,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:54+02:00</t>
-  </si>
-  <si>
-    <t>abc817132da31530</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.bd5d29ee08^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:12+02:00</t>
+  </si>
+  <si>
+    <t>2196e8b9d75f4b00</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a9825820ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT14_KO</t>
@@ -1052,13 +1052,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:55:57+02:00</t>
-  </si>
-  <si>
-    <t>8a3bee0f3b623b69</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.a1a4415591^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:14+02:00</t>
+  </si>
+  <si>
+    <t>4e5da9a00851ab58</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.399ecbb8e4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT15_KO</t>
@@ -1068,13 +1068,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:56:00+02:00</t>
-  </si>
-  <si>
-    <t>ac9786fa7456289d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.5eab687991^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:15+02:00</t>
+  </si>
+  <si>
+    <t>b4979cd83d6cdf79</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.3410d6ad6b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT16_KO</t>
@@ -1084,13 +1084,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:56:03+02:00</t>
-  </si>
-  <si>
-    <t>bc9634491700430c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.f094a7a94d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:16+02:00</t>
+  </si>
+  <si>
+    <t>8fc1940bb1f8d942</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.ef0bb6dcaa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT5_KO</t>
@@ -1101,13 +1101,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-22T08:56:06+02:00</t>
-  </si>
-  <si>
-    <t>26c969746b5d4b2a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.752148eb17^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:17+02:00</t>
+  </si>
+  <si>
+    <t>38d9942af6d76e95</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.dbb02002d7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT6_KO</t>
@@ -1126,13 +1126,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-22T08:56:09+02:00</t>
-  </si>
-  <si>
-    <t>09d680fff5421349</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.734d641789^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:19+02:00</t>
+  </si>
+  <si>
+    <t>f77122ca8ed0e543</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.503c09df8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT8_KO</t>
@@ -1143,13 +1143,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-22T08:56:12+02:00</t>
-  </si>
-  <si>
-    <t>0db1f9441993332e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.158a6a5850^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:20+02:00</t>
+  </si>
+  <si>
+    <t>74406891c341edf1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.486058f571^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT9_KO</t>
@@ -1160,13 +1160,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-22T08:56:15+02:00</t>
-  </si>
-  <si>
-    <t>5407f62d417de31a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.e4a6239e5b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:21+02:00</t>
+  </si>
+  <si>
+    <t>b8978a62c57d2959</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.a470d2c262^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT10_KO</t>
@@ -1177,13 +1177,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-22T08:56:18+02:00</t>
-  </si>
-  <si>
-    <t>59dbd493c9e0a7ef</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.860e734981^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:22+02:00</t>
+  </si>
+  <si>
+    <t>510b6bc8d419aade</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.ed01ab2d03^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT11_KO</t>
@@ -1194,13 +1194,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-22T08:56:21+02:00</t>
-  </si>
-  <si>
-    <t>bea8bf3d43422d49</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.5c33390d7f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:24+02:00</t>
+  </si>
+  <si>
+    <t>8afa3df7006277d4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.4df2c1dffa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT12_KO</t>
@@ -1211,13 +1211,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-22T08:56:24+02:00</t>
-  </si>
-  <si>
-    <t>cfbfb2d894fe559e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.8e18217075^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:25+02:00</t>
+  </si>
+  <si>
+    <t>952f5c51cb627b7c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.44bdde5edb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT13_KO</t>
@@ -1228,13 +1228,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-22T08:56:27+02:00</t>
-  </si>
-  <si>
-    <t>dd7c1626a0dda725</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.7864fa584c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:26+02:00</t>
+  </si>
+  <si>
+    <t>36f6185beb43ff2e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.f52c32e002^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT14_KO</t>
@@ -1245,13 +1245,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-22T08:56:30+02:00</t>
-  </si>
-  <si>
-    <t>4cac115d5fe5f91c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.ba0a2529c6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:28+02:00</t>
+  </si>
+  <si>
+    <t>ab0b2e62e7a6c67b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.7115fb5bf6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT15_KO</t>
@@ -1262,13 +1262,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-22T08:56:33+02:00</t>
-  </si>
-  <si>
-    <t>bc204637e6b47dbc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.f01be87372^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:29+02:00</t>
+  </si>
+  <si>
+    <t>fc22432f8cfb3eb5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.e1bf252d71^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT16_KO</t>
@@ -1279,13 +1279,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2023-08-22T08:56:36+02:00</t>
-  </si>
-  <si>
-    <t>6c02f515f1dc5250</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.e26ea0370b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:30+02:00</t>
+  </si>
+  <si>
+    <t>b96154b043d3a01d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.b7fe8e3f14^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT5_KO</t>
@@ -1296,13 +1296,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:56:39+02:00</t>
-  </si>
-  <si>
-    <t>f61de6cf7e294dd3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.3f5263378e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:31+02:00</t>
+  </si>
+  <si>
+    <t>cd68a03d1f2984b9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.bba88e3edf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT6_KO</t>
@@ -1320,13 +1320,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:56:41+02:00</t>
-  </si>
-  <si>
-    <t>e2242e1c44a81048</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.fe1c3552bd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:33+02:00</t>
+  </si>
+  <si>
+    <t>1c4802c482db8d39</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.0f3df8114d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT8_KO</t>
@@ -1336,13 +1336,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:56:45+02:00</t>
-  </si>
-  <si>
-    <t>90f75243211e6d1c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d021e1ea3e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:34+02:00</t>
+  </si>
+  <si>
+    <t>ae7730e1dc085e7c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.56352ba09c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT9_KO</t>
@@ -1353,13 +1353,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:56:48+02:00</t>
-  </si>
-  <si>
-    <t>1d1464afc54cf501</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.7db2ab2074^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:35+02:00</t>
+  </si>
+  <si>
+    <t>0bd42197a31062c4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.aa25bc92eb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT10_KO</t>
@@ -1370,13 +1370,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:56:51+02:00</t>
-  </si>
-  <si>
-    <t>4fdc019fcd138828</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b17c94cd65^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:37+02:00</t>
+  </si>
+  <si>
+    <t>3a6d725d6e42f7e8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.443d39c655^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT11_KO</t>
@@ -1387,13 +1387,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:56:54+02:00</t>
-  </si>
-  <si>
-    <t>524e2445f2eb7252</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.c95bc7d7e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:38+02:00</t>
+  </si>
+  <si>
+    <t>21e10e80ff08dd21</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.02bcdf5696^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT12_KO</t>
@@ -1404,13 +1404,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:56:57+02:00</t>
-  </si>
-  <si>
-    <t>192370ec22952ab9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.86251ac75e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:39+02:00</t>
+  </si>
+  <si>
+    <t>923c64ed06e73973</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d659c09e4c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT13_KO</t>
@@ -1420,13 +1420,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:00+02:00</t>
-  </si>
-  <si>
-    <t>9a2f16c3c7bc87ad</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.97ca206309^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:40+02:00</t>
+  </si>
+  <si>
+    <t>6781b2ec4cb64189</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.f36c49dfcd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT14_KO</t>
@@ -1436,13 +1436,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:03+02:00</t>
-  </si>
-  <si>
-    <t>e99e84486731f1ae</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b4f244a801^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:42+02:00</t>
+  </si>
+  <si>
+    <t>667efa59149cc2a0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.ed84903a1a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT15_KO</t>
@@ -1453,13 +1453,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:06+02:00</t>
-  </si>
-  <si>
-    <t>3d5df5feb25a9eca</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.70204ed3d9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:43+02:00</t>
+  </si>
+  <si>
+    <t>0704d86f98b39000</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.b34f5d6df7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT16_KO</t>
@@ -1470,13 +1470,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:09+02:00</t>
-  </si>
-  <si>
-    <t>eafd47e8bbc15911</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.a4a94b0a63^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:44+02:00</t>
+  </si>
+  <si>
+    <t>8b2f13aa2766a24a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.ae6fbeff4d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT17_KO</t>
@@ -1487,13 +1487,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:12+02:00</t>
-  </si>
-  <si>
-    <t>76c34d46fe2bc2b1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.5ba2e4d808^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:45+02:00</t>
+  </si>
+  <si>
+    <t>6867df9a2cd8074a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.c2506f41c6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT18_KO</t>
@@ -1504,13 +1504,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:15+02:00</t>
-  </si>
-  <si>
-    <t>fc2d006fd826747c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.d1b2ff41ad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:47+02:00</t>
+  </si>
+  <si>
+    <t>cf0ee75c4dc8f714</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.af0529ee88^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT19_KO</t>
@@ -1520,13 +1520,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:18+02:00</t>
-  </si>
-  <si>
-    <t>f075012576ec8e5c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.64c642b4b6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:48+02:00</t>
+  </si>
+  <si>
+    <t>ebf3732c5d0ddbf0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.84c1683b49^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT20_KO</t>
@@ -1536,13 +1536,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:22+02:00</t>
-  </si>
-  <si>
-    <t>e43d30883ed1e1e3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.0ddcc4a2ff^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:49+02:00</t>
+  </si>
+  <si>
+    <t>7c7a3bf519f9fc20</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.0d27c9fb98^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT21_KO</t>
@@ -1553,13 +1553,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:25+02:00</t>
-  </si>
-  <si>
-    <t>0e27e3dec7337175</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.8be1accccb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:51+02:00</t>
+  </si>
+  <si>
+    <t>24138dfa60ecd0a8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.4cd20acb99^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT22_KO</t>
@@ -1570,13 +1570,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:28+02:00</t>
-  </si>
-  <si>
-    <t>08b78847030146d0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.0418c1cb11^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:52+02:00</t>
+  </si>
+  <si>
+    <t>ecf3737eb2db5bca</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.dd587f850b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT23_KO</t>
@@ -1587,13 +1587,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:31+02:00</t>
-  </si>
-  <si>
-    <t>51a11fd8b03f5394</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.72ca2e24bc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:53+02:00</t>
+  </si>
+  <si>
+    <t>005c7fc7fc17596d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.4b3216daca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT5_KO</t>
@@ -2007,13 +2007,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-22T08:58:29+02:00</t>
-  </si>
-  <si>
-    <t>3bc0ce383136953f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5daaaf4fbf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:19+02:00</t>
+  </si>
+  <si>
+    <t>81846d476a220086</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.711e6bb803^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT2</t>
@@ -2025,13 +2025,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-22T08:58:33+02:00</t>
-  </si>
-  <si>
-    <t>c8f31890112d5054</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.b07ab7b7da^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:20+02:00</t>
+  </si>
+  <si>
+    <t>bce17336eec09362</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.3b43ec7d9f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT3</t>
@@ -2043,13 +2043,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-22T08:58:36+02:00</t>
-  </si>
-  <si>
-    <t>5c825099182ed331</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.3bdb8a18c8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:21+02:00</t>
+  </si>
+  <si>
+    <t>d7599aab22d9ae91</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.6c2980ecd6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT4</t>
@@ -2061,13 +2061,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-22T08:58:39+02:00</t>
-  </si>
-  <si>
-    <t>e88968e93166958e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.0abf125a24^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:22+02:00</t>
+  </si>
+  <si>
+    <t>4217384b00b41ec1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.3dede24a33^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT5_KO</t>
@@ -2077,13 +2077,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:34+02:00</t>
-  </si>
-  <si>
-    <t>84b96ff5c469b1f1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.0870375500^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:55+02:00</t>
+  </si>
+  <si>
+    <t>7b619fb05d8c55e4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.a75b723064^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT6_KO</t>
@@ -2102,13 +2102,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:37+02:00</t>
-  </si>
-  <si>
-    <t>b9bbcf5abe9605d3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.6493759e2d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:56+02:00</t>
+  </si>
+  <si>
+    <t>f1c083207ae31420</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.10b79be6fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT8_KO</t>
@@ -2119,13 +2119,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:40+02:00</t>
-  </si>
-  <si>
-    <t>05364ced6df7e5c5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.af4e89df39^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:57+02:00</t>
+  </si>
+  <si>
+    <t>d7c7462cb4911e57</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.615bf2fe35^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT9_KO</t>
@@ -2136,13 +2136,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:43+02:00</t>
-  </si>
-  <si>
-    <t>acd7448c639a2fdd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.08e3280f8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:08:59+02:00</t>
+  </si>
+  <si>
+    <t>1ccb2dd392306f19</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.11ec9b7ba2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT10_KO</t>
@@ -2153,13 +2153,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:47+02:00</t>
-  </si>
-  <si>
-    <t>1e549c4dc1a58af8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.ad7bfb099c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:00+02:00</t>
+  </si>
+  <si>
+    <t>daaf302c31112208</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.73a67f4a1c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT11_KO</t>
@@ -2170,13 +2170,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:50+02:00</t>
-  </si>
-  <si>
-    <t>fa4317f69f47f30b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.f52ffcd376^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:01+02:00</t>
+  </si>
+  <si>
+    <t>e34105607156ffea</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5ba1b1b7df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT12_KO</t>
@@ -2187,13 +2187,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:52+02:00</t>
-  </si>
-  <si>
-    <t>5452d47079dba473</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.a1a86dd04e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:02+02:00</t>
+  </si>
+  <si>
+    <t>7c6636ef93efbd47</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.784eac1ccf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT13_KO</t>
@@ -2203,13 +2203,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:55+02:00</t>
-  </si>
-  <si>
-    <t>793825fa178a130c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.86605d107b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:04+02:00</t>
+  </si>
+  <si>
+    <t>0d85e02b2b09d3a5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.057b9b5fa0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT14_KO</t>
@@ -2219,13 +2219,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:57:59+02:00</t>
-  </si>
-  <si>
-    <t>5cb4988c572bcd61</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c1a75b97a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:06+02:00</t>
+  </si>
+  <si>
+    <t>9d8c413cb6efc61a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.1c550d84a2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT15_KO</t>
@@ -2236,13 +2236,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:58:02+02:00</t>
-  </si>
-  <si>
-    <t>b7b2c243378503f1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.33224f5d0d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:07+02:00</t>
+  </si>
+  <si>
+    <t>fed897e46d10af65</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.d6b9db3336^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT16_KO</t>
@@ -2253,13 +2253,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:58:05+02:00</t>
-  </si>
-  <si>
-    <t>74e84c0bd544d956</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5614842fef^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:08+02:00</t>
+  </si>
+  <si>
+    <t>af03bf7930c7eb54</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.e6faa99416^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT17_KO</t>
@@ -2270,13 +2270,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:58:08+02:00</t>
-  </si>
-  <si>
-    <t>ec4d503b52880f97</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c0fb5cbcd9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:09+02:00</t>
+  </si>
+  <si>
+    <t>6c7089f77c640af4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.5a040d4a8d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT18_KO</t>
@@ -2287,13 +2287,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:58:11+02:00</t>
-  </si>
-  <si>
-    <t>1d89126b3fa41bfd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c0895d9d89^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:11+02:00</t>
+  </si>
+  <si>
+    <t>853b6c9b7b83ddc2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.9293dd4f6e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT19_KO</t>
@@ -2304,13 +2304,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:58:14+02:00</t>
-  </si>
-  <si>
-    <t>264469fc074ff0ad</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.1d78515aef^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:12+02:00</t>
+  </si>
+  <si>
+    <t>8ac12d12ba4c36d6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.2b3a78e58d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT20_KO</t>
@@ -2321,13 +2321,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:58:17+02:00</t>
-  </si>
-  <si>
-    <t>7ee1a26fe6211fea</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c9f5b43437^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:13+02:00</t>
+  </si>
+  <si>
+    <t>0e07e97689d74ced</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.92f89d58d6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT21_KO</t>
@@ -2338,13 +2338,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:58:20+02:00</t>
-  </si>
-  <si>
-    <t>23011ce9977d72d6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c6034ccdf2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:15+02:00</t>
+  </si>
+  <si>
+    <t>d441fbb5f20ab3f3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.db47f232f9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT22_KO</t>
@@ -2355,13 +2355,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:58:23+02:00</t>
-  </si>
-  <si>
-    <t>9739e999c6961ec9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.8ba9c678a7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:16+02:00</t>
+  </si>
+  <si>
+    <t>fa062774a0f27b7b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.bebe1b7cad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT23_KO</t>
@@ -2372,13 +2372,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:58:26+02:00</t>
-  </si>
-  <si>
-    <t>708258d8a4858280</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.fe03afd587^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:17+02:00</t>
+  </si>
+  <si>
+    <t>8e5df9173289d8be</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.55a38642b6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_PSS_CT1</t>
@@ -2560,13 +2560,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-22T08:58:42+02:00</t>
-  </si>
-  <si>
-    <t>6147a06e3f364529</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.6587b68f3c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:24+02:00</t>
+  </si>
+  <si>
+    <t>d0398febfdea4998</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.d645b17332^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>PUBBLICAZIONE_CREAZIONE</t>
@@ -4560,13 +4560,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-22T08:58:45+02:00</t>
-  </si>
-  <si>
-    <t>c4c10452c03549cc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.deeee125e2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:25+02:00</t>
+  </si>
+  <si>
+    <t>f6fb76f58701deb3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.d5d6a4ad3f4e9de3844e5adf8648a3f987f893f400e7ddf550d0a9fdabd406c9.847c8e3aa1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT0</t>
@@ -4577,13 +4577,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:58:48+02:00</t>
-  </si>
-  <si>
-    <t>c4fc2afafb333599</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.27261d7251^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:26+02:00</t>
+  </si>
+  <si>
+    <t>ef8dfc0d58b3db80</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.cd8380de22641cee2d43e8eba05481546b9fc13fee39b1e82f62733ae0f62e33.a96466f444^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT0</t>
@@ -4594,13 +4594,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-08-22T08:58:53+02:00</t>
-  </si>
-  <si>
-    <t>ed4211fb4b8dcf6e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.7837133fd2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:28+02:00</t>
+  </si>
+  <si>
+    <t>9f34a9cd47c14a32</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8fe46b71d98546dc779f4a7f4859b056b254bbe56b59baa550333b2c46441c87.76c9351a7b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_CERT_VAC_CT0</t>
@@ -4636,13 +4636,13 @@
 </t>
   </si>
   <si>
-    <t>2023-08-22T08:58:56+02:00</t>
-  </si>
-  <si>
-    <t>df67496cc406f381</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.14d60e88aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-08-23T16:09:29+02:00</t>
+  </si>
+  <si>
+    <t>8a1bb2e923eacd78</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.752255b1f40dcf8eba1e8ff9cc24f4b5db720992c8d1677b43377d5cfb786eef.c157712d65^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_PSS_CT0</t>

</xml_diff>